<commit_message>
Test chức năng CRUD
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\OneDrive - Hanoi University of Science and Technology\BaiGiang\Quantriduan\DemoTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\National Brother\Documents\GitHub\Qu-n-l-d-n-CNTT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{C2329458-F936-4E58-B5C2-98927AEFA968}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{DA92033F-E7E2-40F0-97C5-4B82ECF31751}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="16" r:id="rId1"/>
@@ -20,17 +19,17 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="H22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="J22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="A23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="H24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="I24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="J24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="A25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -156,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="H26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="I26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -182,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="A27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
   <si>
     <t>Online ID</t>
   </si>
@@ -208,12 +207,6 @@
     <t>Resp</t>
   </si>
   <si>
-    <t>23/08/2008</t>
-  </si>
-  <si>
-    <t>BUG21312</t>
-  </si>
-  <si>
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
@@ -316,24 +309,12 @@
     <t>Not OK</t>
   </si>
   <si>
-    <t>TienND</t>
-  </si>
-  <si>
     <t>Test Date</t>
   </si>
   <si>
     <t>Repairer</t>
   </si>
   <si>
-    <t>AnhDV</t>
-  </si>
-  <si>
-    <t>20/08/2008</t>
-  </si>
-  <si>
-    <t>DinhPX</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -343,37 +324,9 @@
     <t>Related Software:</t>
   </si>
   <si>
-    <t>Xem được phim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Mpeg
-</t>
-  </si>
-  <si>
-    <t>1. Add film mpeg
-2. Mo VLC
-3. Gõ địa chỉ 192.168.0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Không có tham số dòng lệnh
-</t>
-  </si>
-  <si>
-    <t>1. Gõ duy nhất tên chương trình, không có tham số dòng lệnh</t>
-  </si>
-  <si>
     <t>Chạy được</t>
   </si>
   <si>
-    <t>Không có tham số dòng lệnh, nhưng nhập từ Task Manager</t>
-  </si>
-  <si>
-    <t>File Mpeg có thời lượng 3s</t>
-  </si>
-  <si>
-    <t>BUG213</t>
-  </si>
-  <si>
     <t>Tested and result is correct</t>
   </si>
   <si>
@@ -423,12 +376,24 @@
   </si>
   <si>
     <t>Hear and Note</t>
+  </si>
+  <si>
+    <t>HungVV</t>
+  </si>
+  <si>
+    <t>HuyBK</t>
+  </si>
+  <si>
+    <t>Test các chức năng CRUD</t>
+  </si>
+  <si>
+    <t>1. Test các yêu cầu về thêm sửa xóa dữ liệu.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
@@ -1295,6 +1260,30 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1303,30 +1292,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1426,6 +1391,48 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>106493</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>148478</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Hình ảnh 3"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="403412" y="224118"/>
+          <a:ext cx="1081405" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1505,23 +1512,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1557,23 +1547,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1749,14 +1722,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <tabColor indexed="46"/>
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -1801,7 +1774,7 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -1883,7 +1856,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="O6" s="127" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P6" s="127"/>
       <c r="Q6" s="127"/>
@@ -1917,10 +1890,10 @@
       <c r="B9" s="30"/>
       <c r="C9" s="18"/>
       <c r="D9" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -1931,7 +1904,7 @@
       <c r="B10" s="30"/>
       <c r="C10" s="18"/>
       <c r="D10" s="27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
@@ -1941,7 +1914,7 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="124" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
@@ -1955,34 +1928,34 @@
       <c r="B11" s="30"/>
       <c r="C11" s="18"/>
       <c r="D11" s="31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="128">
         <f ca="1">TODAY()</f>
-        <v>43206</v>
+        <v>43814</v>
       </c>
       <c r="F11" s="128"/>
       <c r="G11" s="128"/>
       <c r="H11" s="82"/>
       <c r="L11" s="33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="V11" s="33"/>
       <c r="X11" s="19"/>
@@ -1990,7 +1963,7 @@
     <row r="12" spans="1:24">
       <c r="B12" s="30"/>
       <c r="L12" s="34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
@@ -2068,7 +2041,7 @@
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E15" s="81"/>
       <c r="F15" s="81"/>
@@ -2199,7 +2172,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
       <c r="L19" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
@@ -2251,7 +2224,7 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E22" s="81"/>
       <c r="F22" s="81"/>
@@ -2278,7 +2251,7 @@
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="L24" s="124" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="M24" s="114"/>
       <c r="N24" s="114"/>
@@ -2413,7 +2386,7 @@
     <row r="31" spans="2:35">
       <c r="B31" s="15"/>
       <c r="C31" s="39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="28"/>
@@ -2449,7 +2422,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2519,7 +2492,7 @@
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
       <c r="C34" s="39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -2555,7 +2528,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2816,14 +2789,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2837,7 +2810,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="65" customFormat="1">
       <c r="A1" s="87" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B1" s="88" t="str">
         <f>Overview!E9</f>
@@ -2848,26 +2821,26 @@
       <c r="E1" s="89"/>
       <c r="F1" s="89"/>
       <c r="G1" s="90" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="H1" s="91" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
         <v>1</v>
       </c>
       <c r="J1" s="92" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="K1" s="93"/>
     </row>
     <row r="2" spans="1:11" s="65" customFormat="1">
       <c r="A2" s="126" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="95"/>
@@ -2875,23 +2848,23 @@
       <c r="F2" s="96"/>
       <c r="G2" s="97"/>
       <c r="H2" s="98" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="I2" s="112">
         <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
       <c r="A3" s="94" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C3" s="95"/>
       <c r="D3" s="95"/>
@@ -2899,14 +2872,14 @@
       <c r="F3" s="96"/>
       <c r="G3" s="97"/>
       <c r="H3" s="98" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="I3" s="113">
         <f>COUNTIF(H2:H787,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="99" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="K3" s="100"/>
     </row>
@@ -2918,7 +2891,7 @@
       <c r="E4" s="96"/>
       <c r="F4" s="96"/>
       <c r="G4" s="102" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H4" s="95"/>
       <c r="I4" s="112">
@@ -2956,10 +2929,10 @@
     </row>
     <row r="7" spans="1:11" ht="10.5" customHeight="1">
       <c r="A7" s="109" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="129" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="129"/>
       <c r="D7" s="129"/>
@@ -2973,49 +2946,49 @@
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="132" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="133"/>
       <c r="D8" s="132" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E8" s="133"/>
       <c r="F8" s="132" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" s="133"/>
       <c r="H8" s="131" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I8" s="131"/>
       <c r="J8" s="48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K8" s="49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="151" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="152"/>
+      <c r="B9" s="150" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="151"/>
       <c r="D9" s="142" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E9" s="143"/>
       <c r="F9" s="51" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="140" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I9" s="141"/>
       <c r="J9" s="50"/>
@@ -3023,39 +2996,41 @@
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="153"/>
-      <c r="C10" s="154"/>
+        <v>32</v>
+      </c>
+      <c r="B10" s="152"/>
+      <c r="C10" s="153"/>
       <c r="D10" s="144"/>
       <c r="E10" s="145"/>
       <c r="F10" s="52"/>
       <c r="G10" s="67"/>
       <c r="H10" s="47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K10" s="138"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="153"/>
-      <c r="C11" s="154"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="152"/>
+      <c r="C11" s="153"/>
       <c r="D11" s="144"/>
       <c r="E11" s="145"/>
       <c r="F11" s="52"/>
       <c r="G11" s="67"/>
       <c r="H11" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="54"/>
+        <v>59</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>60</v>
+      </c>
       <c r="J11" s="50"/>
       <c r="K11" s="138"/>
     </row>
@@ -3063,17 +3038,17 @@
       <c r="A12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
+      <c r="B12" s="152"/>
+      <c r="C12" s="153"/>
       <c r="D12" s="144"/>
       <c r="E12" s="145"/>
       <c r="F12" s="52"/>
       <c r="G12" s="67"/>
       <c r="H12" s="47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J12" s="47"/>
       <c r="K12" s="138"/>
@@ -3082,128 +3057,114 @@
       <c r="A13" s="55">
         <v>981</v>
       </c>
-      <c r="B13" s="155"/>
-      <c r="C13" s="156"/>
+      <c r="B13" s="154"/>
+      <c r="C13" s="155"/>
       <c r="D13" s="146"/>
       <c r="E13" s="147"/>
       <c r="F13" s="56"/>
       <c r="G13" s="68"/>
-      <c r="H13" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="58"/>
+      <c r="H13" s="58">
+        <v>43812</v>
+      </c>
+      <c r="I13" s="58">
+        <v>43812</v>
+      </c>
       <c r="J13" s="59"/>
       <c r="K13" s="139"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="60" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="136"/>
       <c r="D14" s="135" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E14" s="136"/>
       <c r="F14" s="135" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="136"/>
+      <c r="H14" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="158"/>
+      <c r="J14" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="136"/>
-      <c r="H14" s="150" t="s">
+      <c r="K14" s="61" t="s">
         <v>31</v>
-      </c>
-      <c r="I14" s="150"/>
-      <c r="J14" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="61" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="10.5" customHeight="1">
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="151" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="152"/>
-      <c r="D15" s="142" t="s">
-        <v>51</v>
-      </c>
+      <c r="B15" s="150"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="142"/>
       <c r="E15" s="143"/>
-      <c r="F15" s="51" t="s">
-        <v>52</v>
-      </c>
+      <c r="F15" s="51"/>
       <c r="G15" s="66"/>
-      <c r="H15" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I15" s="158"/>
-      <c r="J15" s="57" t="s">
-        <v>3</v>
-      </c>
+      <c r="H15" s="148"/>
+      <c r="I15" s="149"/>
+      <c r="J15" s="57"/>
       <c r="K15" s="137"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="154"/>
+        <v>32</v>
+      </c>
+      <c r="B16" s="152"/>
+      <c r="C16" s="153"/>
       <c r="D16" s="144"/>
       <c r="E16" s="145"/>
       <c r="F16" s="52"/>
       <c r="G16" s="67"/>
       <c r="H16" s="62" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I16" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K16" s="138"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="153"/>
-      <c r="C17" s="154"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="152"/>
+      <c r="C17" s="153"/>
       <c r="D17" s="144"/>
       <c r="E17" s="145"/>
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
-      <c r="H17" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="50"/>
       <c r="K17" s="138"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="153"/>
-      <c r="C18" s="154"/>
+      <c r="B18" s="152"/>
+      <c r="C18" s="153"/>
       <c r="D18" s="144"/>
       <c r="E18" s="145"/>
       <c r="F18" s="52"/>
       <c r="G18" s="67"/>
       <c r="H18" s="62" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="138"/>
@@ -3212,27 +3173,23 @@
       <c r="A19" s="55">
         <v>921</v>
       </c>
-      <c r="B19" s="155"/>
-      <c r="C19" s="156"/>
+      <c r="B19" s="154"/>
+      <c r="C19" s="155"/>
       <c r="D19" s="146"/>
       <c r="E19" s="147"/>
       <c r="F19" s="56"/>
       <c r="G19" s="68"/>
-      <c r="H19" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="54" t="s">
-        <v>2</v>
-      </c>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
       <c r="J19" s="50"/>
       <c r="K19" s="138"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="109" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="134" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="134"/>
       <c r="D20" s="129"/>
@@ -3246,46 +3203,46 @@
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
       <c r="A21" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="148" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="148"/>
-      <c r="D21" s="149"/>
-      <c r="E21" s="149"/>
-      <c r="F21" s="149"/>
-      <c r="G21" s="149"/>
-      <c r="H21" s="149"/>
-      <c r="I21" s="149"/>
-      <c r="J21" s="149"/>
-      <c r="K21" s="149"/>
+        <v>7</v>
+      </c>
+      <c r="B21" s="156" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="156"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157"/>
+      <c r="J21" s="157"/>
+      <c r="K21" s="157"/>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A22" s="62" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="135" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="136"/>
       <c r="D22" s="135" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E22" s="136"/>
       <c r="F22" s="135" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="136"/>
+      <c r="H22" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="158"/>
+      <c r="J22" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="136"/>
-      <c r="H22" s="150" t="s">
+      <c r="K22" s="62" t="s">
         <v>31</v>
-      </c>
-      <c r="I22" s="150"/>
-      <c r="J22" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="62" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
@@ -3293,59 +3250,49 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B23" s="151" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="152"/>
-      <c r="D23" s="142" t="s">
-        <v>49</v>
-      </c>
+      <c r="B23" s="150"/>
+      <c r="C23" s="151"/>
+      <c r="D23" s="142"/>
       <c r="E23" s="143"/>
-      <c r="F23" s="142" t="s">
-        <v>47</v>
-      </c>
+      <c r="F23" s="142"/>
       <c r="G23" s="143"/>
-      <c r="H23" s="140" t="s">
-        <v>37</v>
-      </c>
+      <c r="H23" s="140"/>
       <c r="I23" s="141"/>
       <c r="J23" s="50"/>
       <c r="K23" s="137"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="153"/>
-      <c r="C24" s="154"/>
+        <v>32</v>
+      </c>
+      <c r="B24" s="152"/>
+      <c r="C24" s="153"/>
       <c r="D24" s="144"/>
       <c r="E24" s="145"/>
       <c r="F24" s="144"/>
       <c r="G24" s="145"/>
       <c r="H24" s="62" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I24" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K24" s="138"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="153"/>
-      <c r="C25" s="154"/>
+        <v>12</v>
+      </c>
+      <c r="B25" s="152"/>
+      <c r="C25" s="153"/>
       <c r="D25" s="144"/>
       <c r="E25" s="145"/>
       <c r="F25" s="144"/>
       <c r="G25" s="145"/>
-      <c r="H25" s="54" t="s">
-        <v>43</v>
-      </c>
+      <c r="H25" s="54"/>
       <c r="I25" s="54"/>
       <c r="J25" s="50"/>
       <c r="K25" s="138"/>
@@ -3354,14 +3301,14 @@
       <c r="A26" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="153"/>
-      <c r="C26" s="154"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="153"/>
       <c r="D26" s="144"/>
       <c r="E26" s="145"/>
       <c r="F26" s="144"/>
       <c r="G26" s="145"/>
       <c r="H26" s="62" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I26" s="62"/>
       <c r="J26" s="62"/>
@@ -3371,128 +3318,112 @@
       <c r="A27" s="55">
         <v>922</v>
       </c>
-      <c r="B27" s="155"/>
-      <c r="C27" s="156"/>
+      <c r="B27" s="154"/>
+      <c r="C27" s="155"/>
       <c r="D27" s="146"/>
       <c r="E27" s="147"/>
       <c r="F27" s="146"/>
       <c r="G27" s="147"/>
-      <c r="H27" s="54" t="s">
-        <v>42</v>
-      </c>
+      <c r="H27" s="54"/>
       <c r="I27" s="54"/>
       <c r="J27" s="50"/>
       <c r="K27" s="139"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="132" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="133"/>
       <c r="D28" s="132" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E28" s="133"/>
       <c r="F28" s="132" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G28" s="133"/>
       <c r="H28" s="130" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I28" s="130"/>
       <c r="J28" s="47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K28" s="63" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
       <c r="A29" s="50">
         <v>4</v>
       </c>
-      <c r="B29" s="151" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="152"/>
-      <c r="D29" s="142" t="s">
-        <v>49</v>
-      </c>
+      <c r="B29" s="150"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="142"/>
       <c r="E29" s="143"/>
-      <c r="F29" s="142" t="s">
-        <v>47</v>
-      </c>
+      <c r="F29" s="142"/>
       <c r="G29" s="143"/>
-      <c r="H29" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I29" s="158"/>
-      <c r="J29" s="57" t="s">
-        <v>55</v>
-      </c>
+      <c r="H29" s="148" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="149"/>
+      <c r="J29" s="57"/>
       <c r="K29" s="137"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="153"/>
-      <c r="C30" s="154"/>
+        <v>32</v>
+      </c>
+      <c r="B30" s="152"/>
+      <c r="C30" s="153"/>
       <c r="D30" s="144"/>
       <c r="E30" s="145"/>
       <c r="F30" s="144"/>
       <c r="G30" s="145"/>
       <c r="H30" s="47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I30" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J30" s="47" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K30" s="138"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="153"/>
-      <c r="C31" s="154"/>
+        <v>5</v>
+      </c>
+      <c r="B31" s="152"/>
+      <c r="C31" s="153"/>
       <c r="D31" s="144"/>
       <c r="E31" s="145"/>
       <c r="F31" s="144"/>
       <c r="G31" s="145"/>
-      <c r="H31" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J31" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="50"/>
       <c r="K31" s="138"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="153"/>
-      <c r="C32" s="154"/>
+      <c r="B32" s="152"/>
+      <c r="C32" s="153"/>
       <c r="D32" s="144"/>
       <c r="E32" s="145"/>
       <c r="F32" s="144"/>
       <c r="G32" s="145"/>
       <c r="H32" s="47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I32" s="47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J32" s="47"/>
       <c r="K32" s="138"/>
@@ -3501,130 +3432,110 @@
       <c r="A33" s="55">
         <v>823</v>
       </c>
-      <c r="B33" s="155"/>
-      <c r="C33" s="156"/>
+      <c r="B33" s="154"/>
+      <c r="C33" s="155"/>
       <c r="D33" s="146"/>
       <c r="E33" s="147"/>
       <c r="F33" s="146"/>
       <c r="G33" s="147"/>
-      <c r="H33" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I33" s="54" t="s">
-        <v>2</v>
-      </c>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
       <c r="J33" s="50"/>
       <c r="K33" s="139"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B34" s="132" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C34" s="133"/>
       <c r="D34" s="132" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E34" s="133"/>
       <c r="F34" s="132" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G34" s="133"/>
       <c r="H34" s="130" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I34" s="130"/>
       <c r="J34" s="47" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K34" s="63" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="50">
         <v>5</v>
       </c>
-      <c r="B35" s="151" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="152"/>
-      <c r="D35" s="142" t="s">
-        <v>49</v>
-      </c>
+      <c r="B35" s="150"/>
+      <c r="C35" s="151"/>
+      <c r="D35" s="142"/>
       <c r="E35" s="143"/>
-      <c r="F35" s="142" t="s">
-        <v>47</v>
-      </c>
+      <c r="F35" s="142"/>
       <c r="G35" s="143"/>
-      <c r="H35" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I35" s="158"/>
-      <c r="J35" s="57" t="s">
-        <v>55</v>
-      </c>
+      <c r="H35" s="148"/>
+      <c r="I35" s="149"/>
+      <c r="J35" s="57"/>
       <c r="K35" s="137"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="153"/>
-      <c r="C36" s="154"/>
+        <v>32</v>
+      </c>
+      <c r="B36" s="152"/>
+      <c r="C36" s="153"/>
       <c r="D36" s="144"/>
       <c r="E36" s="145"/>
       <c r="F36" s="144"/>
       <c r="G36" s="145"/>
       <c r="H36" s="47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I36" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J36" s="47" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K36" s="138"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="153"/>
-      <c r="C37" s="154"/>
+        <v>5</v>
+      </c>
+      <c r="B37" s="152"/>
+      <c r="C37" s="153"/>
       <c r="D37" s="144"/>
       <c r="E37" s="145"/>
       <c r="F37" s="144"/>
       <c r="G37" s="145"/>
-      <c r="H37" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="50" t="s">
-        <v>38</v>
-      </c>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="50"/>
       <c r="K37" s="138"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="153"/>
-      <c r="C38" s="154"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="153"/>
       <c r="D38" s="144"/>
       <c r="E38" s="145"/>
       <c r="F38" s="144"/>
       <c r="G38" s="145"/>
       <c r="H38" s="47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I38" s="47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J38" s="47"/>
       <c r="K38" s="138"/>
@@ -3633,18 +3544,14 @@
       <c r="A39" s="55">
         <v>823</v>
       </c>
-      <c r="B39" s="155"/>
-      <c r="C39" s="156"/>
+      <c r="B39" s="154"/>
+      <c r="C39" s="155"/>
       <c r="D39" s="146"/>
       <c r="E39" s="147"/>
       <c r="F39" s="146"/>
       <c r="G39" s="147"/>
-      <c r="H39" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I39" s="54" t="s">
-        <v>2</v>
-      </c>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
       <c r="J39" s="50"/>
       <c r="K39" s="139"/>
     </row>
@@ -4049,17 +3956,15 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B29:C33"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C13"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
     <mergeCell ref="B35:C39"/>
     <mergeCell ref="D29:E33"/>
     <mergeCell ref="D35:E39"/>
@@ -4068,17 +3973,19 @@
     <mergeCell ref="D9:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B21:K21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="B23:C27"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D15:E19"/>
     <mergeCell ref="B15:C19"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="F29:G33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H8:I8"/>

</xml_diff>

<commit_message>
Revert "Test chức năng CRUD"
This reverts commit 79f65a8aa55074e048daed8371a1fbb7b1f46720.
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\National Brother\Documents\GitHub\Qu-n-l-d-n-CNTT\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\OneDrive - Hanoi University of Science and Technology\BaiGiang\Quantriduan\DemoTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{C2329458-F936-4E58-B5C2-98927AEFA968}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{DA92033F-E7E2-40F0-97C5-4B82ECF31751}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="16" r:id="rId1"/>
@@ -19,17 +20,17 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -43,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0">
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0">
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0">
+    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I24" authorId="0" shapeId="0">
+    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0">
+    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0">
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="0" shapeId="0">
+    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="0" shapeId="0">
+    <comment ref="I26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -199,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
   <si>
     <t>Online ID</t>
   </si>
@@ -207,6 +208,12 @@
     <t>Resp</t>
   </si>
   <si>
+    <t>23/08/2008</t>
+  </si>
+  <si>
+    <t>BUG21312</t>
+  </si>
+  <si>
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
@@ -309,12 +316,24 @@
     <t>Not OK</t>
   </si>
   <si>
+    <t>TienND</t>
+  </si>
+  <si>
     <t>Test Date</t>
   </si>
   <si>
     <t>Repairer</t>
   </si>
   <si>
+    <t>AnhDV</t>
+  </si>
+  <si>
+    <t>20/08/2008</t>
+  </si>
+  <si>
+    <t>DinhPX</t>
+  </si>
+  <si>
     <t>OK</t>
   </si>
   <si>
@@ -324,9 +343,37 @@
     <t>Related Software:</t>
   </si>
   <si>
+    <t>Xem được phim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Mpeg
+</t>
+  </si>
+  <si>
+    <t>1. Add film mpeg
+2. Mo VLC
+3. Gõ địa chỉ 192.168.0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Không có tham số dòng lệnh
+</t>
+  </si>
+  <si>
+    <t>1. Gõ duy nhất tên chương trình, không có tham số dòng lệnh</t>
+  </si>
+  <si>
     <t>Chạy được</t>
   </si>
   <si>
+    <t>Không có tham số dòng lệnh, nhưng nhập từ Task Manager</t>
+  </si>
+  <si>
+    <t>File Mpeg có thời lượng 3s</t>
+  </si>
+  <si>
+    <t>BUG213</t>
+  </si>
+  <si>
     <t>Tested and result is correct</t>
   </si>
   <si>
@@ -376,24 +423,12 @@
   </si>
   <si>
     <t>Hear and Note</t>
-  </si>
-  <si>
-    <t>HungVV</t>
-  </si>
-  <si>
-    <t>HuyBK</t>
-  </si>
-  <si>
-    <t>Test các chức năng CRUD</t>
-  </si>
-  <si>
-    <t>1. Test các yêu cầu về thêm sửa xóa dữ liệu.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
@@ -1260,38 +1295,38 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1391,48 +1426,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>302559</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>56030</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>106493</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>148478</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Hình ảnh 3"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="403412" y="224118"/>
-          <a:ext cx="1081405" cy="809625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1512,6 +1505,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1547,6 +1557,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1722,14 +1749,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor indexed="46"/>
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -1774,7 +1801,7 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -1856,7 +1883,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="O6" s="127" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P6" s="127"/>
       <c r="Q6" s="127"/>
@@ -1890,10 +1917,10 @@
       <c r="B9" s="30"/>
       <c r="C9" s="18"/>
       <c r="D9" s="27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -1904,7 +1931,7 @@
       <c r="B10" s="30"/>
       <c r="C10" s="18"/>
       <c r="D10" s="27" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
@@ -1914,7 +1941,7 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="124" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
@@ -1928,34 +1955,34 @@
       <c r="B11" s="30"/>
       <c r="C11" s="18"/>
       <c r="D11" s="31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11" s="128">
         <f ca="1">TODAY()</f>
-        <v>43814</v>
+        <v>43206</v>
       </c>
       <c r="F11" s="128"/>
       <c r="G11" s="128"/>
       <c r="H11" s="82"/>
       <c r="L11" s="33" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="V11" s="33"/>
       <c r="X11" s="19"/>
@@ -1963,7 +1990,7 @@
     <row r="12" spans="1:24">
       <c r="B12" s="30"/>
       <c r="L12" s="34" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
@@ -2041,7 +2068,7 @@
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E15" s="81"/>
       <c r="F15" s="81"/>
@@ -2172,7 +2199,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
       <c r="L19" s="36" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
@@ -2224,7 +2251,7 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E22" s="81"/>
       <c r="F22" s="81"/>
@@ -2251,7 +2278,7 @@
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="L24" s="124" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="M24" s="114"/>
       <c r="N24" s="114"/>
@@ -2386,7 +2413,7 @@
     <row r="31" spans="2:35">
       <c r="B31" s="15"/>
       <c r="C31" s="39" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="28"/>
@@ -2422,7 +2449,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2492,7 +2519,7 @@
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
       <c r="C34" s="39" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -2528,7 +2555,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2789,14 +2816,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2810,7 +2837,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="65" customFormat="1">
       <c r="A1" s="87" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B1" s="88" t="str">
         <f>Overview!E9</f>
@@ -2821,26 +2848,26 @@
       <c r="E1" s="89"/>
       <c r="F1" s="89"/>
       <c r="G1" s="90" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H1" s="91" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
         <v>1</v>
       </c>
       <c r="J1" s="92" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="K1" s="93"/>
     </row>
     <row r="2" spans="1:11" s="65" customFormat="1">
       <c r="A2" s="126" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="95"/>
@@ -2848,23 +2875,23 @@
       <c r="F2" s="96"/>
       <c r="G2" s="97"/>
       <c r="H2" s="98" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="I2" s="112">
         <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
       <c r="A3" s="94" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="C3" s="95"/>
       <c r="D3" s="95"/>
@@ -2872,14 +2899,14 @@
       <c r="F3" s="96"/>
       <c r="G3" s="97"/>
       <c r="H3" s="98" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="I3" s="113">
         <f>COUNTIF(H2:H787,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="99" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="K3" s="100"/>
     </row>
@@ -2891,7 +2918,7 @@
       <c r="E4" s="96"/>
       <c r="F4" s="96"/>
       <c r="G4" s="102" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="H4" s="95"/>
       <c r="I4" s="112">
@@ -2929,10 +2956,10 @@
     </row>
     <row r="7" spans="1:11" ht="10.5" customHeight="1">
       <c r="A7" s="109" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="129" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="129"/>
       <c r="D7" s="129"/>
@@ -2946,49 +2973,49 @@
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="132" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="133"/>
       <c r="D8" s="132" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E8" s="133"/>
       <c r="F8" s="132" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G8" s="133"/>
       <c r="H8" s="131" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I8" s="131"/>
       <c r="J8" s="48" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" s="49" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="150" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="151"/>
+      <c r="B9" s="151" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="152"/>
       <c r="D9" s="142" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E9" s="143"/>
       <c r="F9" s="51" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="140" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I9" s="141"/>
       <c r="J9" s="50"/>
@@ -2996,41 +3023,39 @@
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="152"/>
-      <c r="C10" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B10" s="153"/>
+      <c r="C10" s="154"/>
       <c r="D10" s="144"/>
       <c r="E10" s="145"/>
       <c r="F10" s="52"/>
       <c r="G10" s="67"/>
       <c r="H10" s="47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K10" s="138"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="152"/>
-      <c r="C11" s="153"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="153"/>
+      <c r="C11" s="154"/>
       <c r="D11" s="144"/>
       <c r="E11" s="145"/>
       <c r="F11" s="52"/>
       <c r="G11" s="67"/>
       <c r="H11" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="54" t="s">
-        <v>60</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="I11" s="54"/>
       <c r="J11" s="50"/>
       <c r="K11" s="138"/>
     </row>
@@ -3038,17 +3063,17 @@
       <c r="A12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="152"/>
-      <c r="C12" s="153"/>
+      <c r="B12" s="153"/>
+      <c r="C12" s="154"/>
       <c r="D12" s="144"/>
       <c r="E12" s="145"/>
       <c r="F12" s="52"/>
       <c r="G12" s="67"/>
       <c r="H12" s="47" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J12" s="47"/>
       <c r="K12" s="138"/>
@@ -3057,114 +3082,128 @@
       <c r="A13" s="55">
         <v>981</v>
       </c>
-      <c r="B13" s="154"/>
-      <c r="C13" s="155"/>
+      <c r="B13" s="155"/>
+      <c r="C13" s="156"/>
       <c r="D13" s="146"/>
       <c r="E13" s="147"/>
       <c r="F13" s="56"/>
       <c r="G13" s="68"/>
-      <c r="H13" s="58">
-        <v>43812</v>
-      </c>
-      <c r="I13" s="58">
-        <v>43812</v>
-      </c>
+      <c r="H13" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="58"/>
       <c r="J13" s="59"/>
       <c r="K13" s="139"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="60" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="136"/>
       <c r="D14" s="135" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E14" s="136"/>
       <c r="F14" s="135" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G14" s="136"/>
-      <c r="H14" s="158" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="158"/>
+      <c r="H14" s="150" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="150"/>
       <c r="J14" s="62" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K14" s="61" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="10.5" customHeight="1">
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="150"/>
-      <c r="C15" s="151"/>
-      <c r="D15" s="142"/>
+      <c r="B15" s="151" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="152"/>
+      <c r="D15" s="142" t="s">
+        <v>51</v>
+      </c>
       <c r="E15" s="143"/>
-      <c r="F15" s="51"/>
+      <c r="F15" s="51" t="s">
+        <v>52</v>
+      </c>
       <c r="G15" s="66"/>
-      <c r="H15" s="148"/>
-      <c r="I15" s="149"/>
-      <c r="J15" s="57"/>
+      <c r="H15" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="158"/>
+      <c r="J15" s="57" t="s">
+        <v>3</v>
+      </c>
       <c r="K15" s="137"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="152"/>
-      <c r="C16" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B16" s="153"/>
+      <c r="C16" s="154"/>
       <c r="D16" s="144"/>
       <c r="E16" s="145"/>
       <c r="F16" s="52"/>
       <c r="G16" s="67"/>
       <c r="H16" s="62" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I16" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K16" s="138"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="152"/>
-      <c r="C17" s="153"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="153"/>
+      <c r="C17" s="154"/>
       <c r="D17" s="144"/>
       <c r="E17" s="145"/>
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="50"/>
+      <c r="H17" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="K17" s="138"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="152"/>
-      <c r="C18" s="153"/>
+      <c r="B18" s="153"/>
+      <c r="C18" s="154"/>
       <c r="D18" s="144"/>
       <c r="E18" s="145"/>
       <c r="F18" s="52"/>
       <c r="G18" s="67"/>
       <c r="H18" s="62" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="138"/>
@@ -3173,23 +3212,27 @@
       <c r="A19" s="55">
         <v>921</v>
       </c>
-      <c r="B19" s="154"/>
-      <c r="C19" s="155"/>
+      <c r="B19" s="155"/>
+      <c r="C19" s="156"/>
       <c r="D19" s="146"/>
       <c r="E19" s="147"/>
       <c r="F19" s="56"/>
       <c r="G19" s="68"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
+      <c r="H19" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="54" t="s">
+        <v>2</v>
+      </c>
       <c r="J19" s="50"/>
       <c r="K19" s="138"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="109" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B20" s="134" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C20" s="134"/>
       <c r="D20" s="129"/>
@@ -3203,46 +3246,46 @@
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
       <c r="A21" s="110" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="156" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="156"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="157"/>
+        <v>9</v>
+      </c>
+      <c r="B21" s="148" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="148"/>
+      <c r="D21" s="149"/>
+      <c r="E21" s="149"/>
+      <c r="F21" s="149"/>
+      <c r="G21" s="149"/>
+      <c r="H21" s="149"/>
+      <c r="I21" s="149"/>
+      <c r="J21" s="149"/>
+      <c r="K21" s="149"/>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A22" s="62" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" s="135" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22" s="136"/>
       <c r="D22" s="135" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E22" s="136"/>
       <c r="F22" s="135" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G22" s="136"/>
-      <c r="H22" s="158" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="158"/>
+      <c r="H22" s="150" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="150"/>
       <c r="J22" s="62" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K22" s="62" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
@@ -3250,49 +3293,59 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B23" s="150"/>
-      <c r="C23" s="151"/>
-      <c r="D23" s="142"/>
+      <c r="B23" s="151" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="152"/>
+      <c r="D23" s="142" t="s">
+        <v>49</v>
+      </c>
       <c r="E23" s="143"/>
-      <c r="F23" s="142"/>
+      <c r="F23" s="142" t="s">
+        <v>47</v>
+      </c>
       <c r="G23" s="143"/>
-      <c r="H23" s="140"/>
+      <c r="H23" s="140" t="s">
+        <v>37</v>
+      </c>
       <c r="I23" s="141"/>
       <c r="J23" s="50"/>
       <c r="K23" s="137"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="152"/>
-      <c r="C24" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B24" s="153"/>
+      <c r="C24" s="154"/>
       <c r="D24" s="144"/>
       <c r="E24" s="145"/>
       <c r="F24" s="144"/>
       <c r="G24" s="145"/>
       <c r="H24" s="62" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I24" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K24" s="138"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="152"/>
-      <c r="C25" s="153"/>
+        <v>14</v>
+      </c>
+      <c r="B25" s="153"/>
+      <c r="C25" s="154"/>
       <c r="D25" s="144"/>
       <c r="E25" s="145"/>
       <c r="F25" s="144"/>
       <c r="G25" s="145"/>
-      <c r="H25" s="54"/>
+      <c r="H25" s="54" t="s">
+        <v>43</v>
+      </c>
       <c r="I25" s="54"/>
       <c r="J25" s="50"/>
       <c r="K25" s="138"/>
@@ -3301,14 +3354,14 @@
       <c r="A26" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="152"/>
-      <c r="C26" s="153"/>
+      <c r="B26" s="153"/>
+      <c r="C26" s="154"/>
       <c r="D26" s="144"/>
       <c r="E26" s="145"/>
       <c r="F26" s="144"/>
       <c r="G26" s="145"/>
       <c r="H26" s="62" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I26" s="62"/>
       <c r="J26" s="62"/>
@@ -3318,112 +3371,128 @@
       <c r="A27" s="55">
         <v>922</v>
       </c>
-      <c r="B27" s="154"/>
-      <c r="C27" s="155"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="156"/>
       <c r="D27" s="146"/>
       <c r="E27" s="147"/>
       <c r="F27" s="146"/>
       <c r="G27" s="147"/>
-      <c r="H27" s="54"/>
+      <c r="H27" s="54" t="s">
+        <v>42</v>
+      </c>
       <c r="I27" s="54"/>
       <c r="J27" s="50"/>
       <c r="K27" s="139"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" s="132" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C28" s="133"/>
       <c r="D28" s="132" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E28" s="133"/>
       <c r="F28" s="132" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G28" s="133"/>
       <c r="H28" s="130" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I28" s="130"/>
       <c r="J28" s="47" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K28" s="63" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
       <c r="A29" s="50">
         <v>4</v>
       </c>
-      <c r="B29" s="150"/>
-      <c r="C29" s="151"/>
-      <c r="D29" s="142"/>
+      <c r="B29" s="151" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="152"/>
+      <c r="D29" s="142" t="s">
+        <v>49</v>
+      </c>
       <c r="E29" s="143"/>
-      <c r="F29" s="142"/>
+      <c r="F29" s="142" t="s">
+        <v>47</v>
+      </c>
       <c r="G29" s="143"/>
-      <c r="H29" s="148" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="149"/>
-      <c r="J29" s="57"/>
+      <c r="H29" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="158"/>
+      <c r="J29" s="57" t="s">
+        <v>55</v>
+      </c>
       <c r="K29" s="137"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="152"/>
-      <c r="C30" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B30" s="153"/>
+      <c r="C30" s="154"/>
       <c r="D30" s="144"/>
       <c r="E30" s="145"/>
       <c r="F30" s="144"/>
       <c r="G30" s="145"/>
       <c r="H30" s="47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I30" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J30" s="47" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K30" s="138"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="152"/>
-      <c r="C31" s="153"/>
+        <v>7</v>
+      </c>
+      <c r="B31" s="153"/>
+      <c r="C31" s="154"/>
       <c r="D31" s="144"/>
       <c r="E31" s="145"/>
       <c r="F31" s="144"/>
       <c r="G31" s="145"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="50"/>
+      <c r="H31" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="K31" s="138"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="152"/>
-      <c r="C32" s="153"/>
+      <c r="B32" s="153"/>
+      <c r="C32" s="154"/>
       <c r="D32" s="144"/>
       <c r="E32" s="145"/>
       <c r="F32" s="144"/>
       <c r="G32" s="145"/>
       <c r="H32" s="47" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I32" s="47" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J32" s="47"/>
       <c r="K32" s="138"/>
@@ -3432,110 +3501,130 @@
       <c r="A33" s="55">
         <v>823</v>
       </c>
-      <c r="B33" s="154"/>
-      <c r="C33" s="155"/>
+      <c r="B33" s="155"/>
+      <c r="C33" s="156"/>
       <c r="D33" s="146"/>
       <c r="E33" s="147"/>
       <c r="F33" s="146"/>
       <c r="G33" s="147"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
+      <c r="H33" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>2</v>
+      </c>
       <c r="J33" s="50"/>
       <c r="K33" s="139"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B34" s="132" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C34" s="133"/>
       <c r="D34" s="132" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E34" s="133"/>
       <c r="F34" s="132" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G34" s="133"/>
       <c r="H34" s="130" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I34" s="130"/>
       <c r="J34" s="47" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K34" s="63" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="50">
         <v>5</v>
       </c>
-      <c r="B35" s="150"/>
-      <c r="C35" s="151"/>
-      <c r="D35" s="142"/>
+      <c r="B35" s="151" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="152"/>
+      <c r="D35" s="142" t="s">
+        <v>49</v>
+      </c>
       <c r="E35" s="143"/>
-      <c r="F35" s="142"/>
+      <c r="F35" s="142" t="s">
+        <v>47</v>
+      </c>
       <c r="G35" s="143"/>
-      <c r="H35" s="148"/>
-      <c r="I35" s="149"/>
-      <c r="J35" s="57"/>
+      <c r="H35" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="158"/>
+      <c r="J35" s="57" t="s">
+        <v>55</v>
+      </c>
       <c r="K35" s="137"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="152"/>
-      <c r="C36" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="153"/>
+      <c r="C36" s="154"/>
       <c r="D36" s="144"/>
       <c r="E36" s="145"/>
       <c r="F36" s="144"/>
       <c r="G36" s="145"/>
       <c r="H36" s="47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I36" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J36" s="47" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K36" s="138"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="152"/>
-      <c r="C37" s="153"/>
+        <v>7</v>
+      </c>
+      <c r="B37" s="153"/>
+      <c r="C37" s="154"/>
       <c r="D37" s="144"/>
       <c r="E37" s="145"/>
       <c r="F37" s="144"/>
       <c r="G37" s="145"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="50"/>
+      <c r="H37" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="J37" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="K37" s="138"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="152"/>
-      <c r="C38" s="153"/>
+      <c r="B38" s="153"/>
+      <c r="C38" s="154"/>
       <c r="D38" s="144"/>
       <c r="E38" s="145"/>
       <c r="F38" s="144"/>
       <c r="G38" s="145"/>
       <c r="H38" s="47" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I38" s="47" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J38" s="47"/>
       <c r="K38" s="138"/>
@@ -3544,14 +3633,18 @@
       <c r="A39" s="55">
         <v>823</v>
       </c>
-      <c r="B39" s="154"/>
-      <c r="C39" s="155"/>
+      <c r="B39" s="155"/>
+      <c r="C39" s="156"/>
       <c r="D39" s="146"/>
       <c r="E39" s="147"/>
       <c r="F39" s="146"/>
       <c r="G39" s="147"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
+      <c r="H39" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="54" t="s">
+        <v>2</v>
+      </c>
       <c r="J39" s="50"/>
       <c r="K39" s="139"/>
     </row>
@@ -3956,15 +4049,17 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H34:I34"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C13"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B29:C33"/>
     <mergeCell ref="B35:C39"/>
     <mergeCell ref="D29:E33"/>
     <mergeCell ref="D35:E39"/>
@@ -3973,19 +4068,17 @@
     <mergeCell ref="D9:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="F29:G33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B21:K21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="B23:C27"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D15:E19"/>
     <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H8:I8"/>

</xml_diff>

<commit_message>
Revert Test chức năng CRUD
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\National Brother\Documents\GitHub\Qu-n-l-d-n-CNTT\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\OneDrive - Hanoi University of Science and Technology\BaiGiang\Quantriduan\DemoTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{C2329458-F936-4E58-B5C2-98927AEFA968}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{DA92033F-E7E2-40F0-97C5-4B82ECF31751}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="16" r:id="rId1"/>
@@ -19,17 +20,17 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -43,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0">
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0">
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0">
+    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I24" authorId="0" shapeId="0">
+    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0">
+    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0">
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="0" shapeId="0">
+    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="0" shapeId="0">
+    <comment ref="I26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -199,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
   <si>
     <t>Online ID</t>
   </si>
@@ -207,6 +208,12 @@
     <t>Resp</t>
   </si>
   <si>
+    <t>23/08/2008</t>
+  </si>
+  <si>
+    <t>BUG21312</t>
+  </si>
+  <si>
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
@@ -309,12 +316,24 @@
     <t>Not OK</t>
   </si>
   <si>
+    <t>TienND</t>
+  </si>
+  <si>
     <t>Test Date</t>
   </si>
   <si>
     <t>Repairer</t>
   </si>
   <si>
+    <t>AnhDV</t>
+  </si>
+  <si>
+    <t>20/08/2008</t>
+  </si>
+  <si>
+    <t>DinhPX</t>
+  </si>
+  <si>
     <t>OK</t>
   </si>
   <si>
@@ -324,9 +343,37 @@
     <t>Related Software:</t>
   </si>
   <si>
+    <t>Xem được phim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Mpeg
+</t>
+  </si>
+  <si>
+    <t>1. Add film mpeg
+2. Mo VLC
+3. Gõ địa chỉ 192.168.0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Không có tham số dòng lệnh
+</t>
+  </si>
+  <si>
+    <t>1. Gõ duy nhất tên chương trình, không có tham số dòng lệnh</t>
+  </si>
+  <si>
     <t>Chạy được</t>
   </si>
   <si>
+    <t>Không có tham số dòng lệnh, nhưng nhập từ Task Manager</t>
+  </si>
+  <si>
+    <t>File Mpeg có thời lượng 3s</t>
+  </si>
+  <si>
+    <t>BUG213</t>
+  </si>
+  <si>
     <t>Tested and result is correct</t>
   </si>
   <si>
@@ -376,24 +423,12 @@
   </si>
   <si>
     <t>Hear and Note</t>
-  </si>
-  <si>
-    <t>HungVV</t>
-  </si>
-  <si>
-    <t>HuyBK</t>
-  </si>
-  <si>
-    <t>Test các chức năng CRUD</t>
-  </si>
-  <si>
-    <t>1. Test các yêu cầu về thêm sửa xóa dữ liệu.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
@@ -1260,38 +1295,38 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1391,48 +1426,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>302559</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>56030</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>106493</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>148478</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Hình ảnh 3"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="403412" y="224118"/>
-          <a:ext cx="1081405" cy="809625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1512,6 +1505,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1547,6 +1557,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1722,14 +1749,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor indexed="46"/>
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -1774,7 +1801,7 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -1856,7 +1883,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="O6" s="127" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P6" s="127"/>
       <c r="Q6" s="127"/>
@@ -1890,10 +1917,10 @@
       <c r="B9" s="30"/>
       <c r="C9" s="18"/>
       <c r="D9" s="27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -1904,7 +1931,7 @@
       <c r="B10" s="30"/>
       <c r="C10" s="18"/>
       <c r="D10" s="27" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
@@ -1914,7 +1941,7 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="124" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
@@ -1928,34 +1955,34 @@
       <c r="B11" s="30"/>
       <c r="C11" s="18"/>
       <c r="D11" s="31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11" s="128">
         <f ca="1">TODAY()</f>
-        <v>43814</v>
+        <v>43206</v>
       </c>
       <c r="F11" s="128"/>
       <c r="G11" s="128"/>
       <c r="H11" s="82"/>
       <c r="L11" s="33" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="V11" s="33"/>
       <c r="X11" s="19"/>
@@ -1963,7 +1990,7 @@
     <row r="12" spans="1:24">
       <c r="B12" s="30"/>
       <c r="L12" s="34" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
@@ -2041,7 +2068,7 @@
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E15" s="81"/>
       <c r="F15" s="81"/>
@@ -2172,7 +2199,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
       <c r="L19" s="36" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
@@ -2224,7 +2251,7 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E22" s="81"/>
       <c r="F22" s="81"/>
@@ -2251,7 +2278,7 @@
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="L24" s="124" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="M24" s="114"/>
       <c r="N24" s="114"/>
@@ -2386,7 +2413,7 @@
     <row r="31" spans="2:35">
       <c r="B31" s="15"/>
       <c r="C31" s="39" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="28"/>
@@ -2422,7 +2449,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2492,7 +2519,7 @@
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
       <c r="C34" s="39" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -2528,7 +2555,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2789,14 +2816,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2810,7 +2837,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="65" customFormat="1">
       <c r="A1" s="87" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B1" s="88" t="str">
         <f>Overview!E9</f>
@@ -2821,26 +2848,26 @@
       <c r="E1" s="89"/>
       <c r="F1" s="89"/>
       <c r="G1" s="90" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H1" s="91" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
         <v>1</v>
       </c>
       <c r="J1" s="92" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="K1" s="93"/>
     </row>
     <row r="2" spans="1:11" s="65" customFormat="1">
       <c r="A2" s="126" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="95"/>
@@ -2848,23 +2875,23 @@
       <c r="F2" s="96"/>
       <c r="G2" s="97"/>
       <c r="H2" s="98" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="I2" s="112">
         <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
       <c r="A3" s="94" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="C3" s="95"/>
       <c r="D3" s="95"/>
@@ -2872,14 +2899,14 @@
       <c r="F3" s="96"/>
       <c r="G3" s="97"/>
       <c r="H3" s="98" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="I3" s="113">
         <f>COUNTIF(H2:H787,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="99" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="K3" s="100"/>
     </row>
@@ -2891,7 +2918,7 @@
       <c r="E4" s="96"/>
       <c r="F4" s="96"/>
       <c r="G4" s="102" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="H4" s="95"/>
       <c r="I4" s="112">
@@ -2929,10 +2956,10 @@
     </row>
     <row r="7" spans="1:11" ht="10.5" customHeight="1">
       <c r="A7" s="109" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="129" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="129"/>
       <c r="D7" s="129"/>
@@ -2946,49 +2973,49 @@
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="132" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="133"/>
       <c r="D8" s="132" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E8" s="133"/>
       <c r="F8" s="132" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G8" s="133"/>
       <c r="H8" s="131" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I8" s="131"/>
       <c r="J8" s="48" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K8" s="49" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="150" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="151"/>
+      <c r="B9" s="151" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="152"/>
       <c r="D9" s="142" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E9" s="143"/>
       <c r="F9" s="51" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="140" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I9" s="141"/>
       <c r="J9" s="50"/>
@@ -2996,41 +3023,39 @@
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="152"/>
-      <c r="C10" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B10" s="153"/>
+      <c r="C10" s="154"/>
       <c r="D10" s="144"/>
       <c r="E10" s="145"/>
       <c r="F10" s="52"/>
       <c r="G10" s="67"/>
       <c r="H10" s="47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K10" s="138"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="152"/>
-      <c r="C11" s="153"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="153"/>
+      <c r="C11" s="154"/>
       <c r="D11" s="144"/>
       <c r="E11" s="145"/>
       <c r="F11" s="52"/>
       <c r="G11" s="67"/>
       <c r="H11" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="54" t="s">
-        <v>60</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="I11" s="54"/>
       <c r="J11" s="50"/>
       <c r="K11" s="138"/>
     </row>
@@ -3038,17 +3063,17 @@
       <c r="A12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="152"/>
-      <c r="C12" s="153"/>
+      <c r="B12" s="153"/>
+      <c r="C12" s="154"/>
       <c r="D12" s="144"/>
       <c r="E12" s="145"/>
       <c r="F12" s="52"/>
       <c r="G12" s="67"/>
       <c r="H12" s="47" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J12" s="47"/>
       <c r="K12" s="138"/>
@@ -3057,114 +3082,128 @@
       <c r="A13" s="55">
         <v>981</v>
       </c>
-      <c r="B13" s="154"/>
-      <c r="C13" s="155"/>
+      <c r="B13" s="155"/>
+      <c r="C13" s="156"/>
       <c r="D13" s="146"/>
       <c r="E13" s="147"/>
       <c r="F13" s="56"/>
       <c r="G13" s="68"/>
-      <c r="H13" s="58">
-        <v>43812</v>
-      </c>
-      <c r="I13" s="58">
-        <v>43812</v>
-      </c>
+      <c r="H13" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="58"/>
       <c r="J13" s="59"/>
       <c r="K13" s="139"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="60" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="136"/>
       <c r="D14" s="135" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E14" s="136"/>
       <c r="F14" s="135" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G14" s="136"/>
-      <c r="H14" s="158" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="158"/>
+      <c r="H14" s="150" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="150"/>
       <c r="J14" s="62" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K14" s="61" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="10.5" customHeight="1">
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="150"/>
-      <c r="C15" s="151"/>
-      <c r="D15" s="142"/>
+      <c r="B15" s="151" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="152"/>
+      <c r="D15" s="142" t="s">
+        <v>51</v>
+      </c>
       <c r="E15" s="143"/>
-      <c r="F15" s="51"/>
+      <c r="F15" s="51" t="s">
+        <v>52</v>
+      </c>
       <c r="G15" s="66"/>
-      <c r="H15" s="148"/>
-      <c r="I15" s="149"/>
-      <c r="J15" s="57"/>
+      <c r="H15" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="158"/>
+      <c r="J15" s="57" t="s">
+        <v>3</v>
+      </c>
       <c r="K15" s="137"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="152"/>
-      <c r="C16" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B16" s="153"/>
+      <c r="C16" s="154"/>
       <c r="D16" s="144"/>
       <c r="E16" s="145"/>
       <c r="F16" s="52"/>
       <c r="G16" s="67"/>
       <c r="H16" s="62" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I16" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K16" s="138"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="152"/>
-      <c r="C17" s="153"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="153"/>
+      <c r="C17" s="154"/>
       <c r="D17" s="144"/>
       <c r="E17" s="145"/>
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="50"/>
+      <c r="H17" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="K17" s="138"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="152"/>
-      <c r="C18" s="153"/>
+      <c r="B18" s="153"/>
+      <c r="C18" s="154"/>
       <c r="D18" s="144"/>
       <c r="E18" s="145"/>
       <c r="F18" s="52"/>
       <c r="G18" s="67"/>
       <c r="H18" s="62" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="138"/>
@@ -3173,23 +3212,27 @@
       <c r="A19" s="55">
         <v>921</v>
       </c>
-      <c r="B19" s="154"/>
-      <c r="C19" s="155"/>
+      <c r="B19" s="155"/>
+      <c r="C19" s="156"/>
       <c r="D19" s="146"/>
       <c r="E19" s="147"/>
       <c r="F19" s="56"/>
       <c r="G19" s="68"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
+      <c r="H19" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="54" t="s">
+        <v>2</v>
+      </c>
       <c r="J19" s="50"/>
       <c r="K19" s="138"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="109" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B20" s="134" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C20" s="134"/>
       <c r="D20" s="129"/>
@@ -3203,46 +3246,46 @@
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
       <c r="A21" s="110" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="156" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="156"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="157"/>
+        <v>9</v>
+      </c>
+      <c r="B21" s="148" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="148"/>
+      <c r="D21" s="149"/>
+      <c r="E21" s="149"/>
+      <c r="F21" s="149"/>
+      <c r="G21" s="149"/>
+      <c r="H21" s="149"/>
+      <c r="I21" s="149"/>
+      <c r="J21" s="149"/>
+      <c r="K21" s="149"/>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A22" s="62" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" s="135" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C22" s="136"/>
       <c r="D22" s="135" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E22" s="136"/>
       <c r="F22" s="135" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G22" s="136"/>
-      <c r="H22" s="158" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="158"/>
+      <c r="H22" s="150" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="150"/>
       <c r="J22" s="62" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K22" s="62" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
@@ -3250,49 +3293,59 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B23" s="150"/>
-      <c r="C23" s="151"/>
-      <c r="D23" s="142"/>
+      <c r="B23" s="151" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="152"/>
+      <c r="D23" s="142" t="s">
+        <v>49</v>
+      </c>
       <c r="E23" s="143"/>
-      <c r="F23" s="142"/>
+      <c r="F23" s="142" t="s">
+        <v>47</v>
+      </c>
       <c r="G23" s="143"/>
-      <c r="H23" s="140"/>
+      <c r="H23" s="140" t="s">
+        <v>37</v>
+      </c>
       <c r="I23" s="141"/>
       <c r="J23" s="50"/>
       <c r="K23" s="137"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="152"/>
-      <c r="C24" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B24" s="153"/>
+      <c r="C24" s="154"/>
       <c r="D24" s="144"/>
       <c r="E24" s="145"/>
       <c r="F24" s="144"/>
       <c r="G24" s="145"/>
       <c r="H24" s="62" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I24" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K24" s="138"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="152"/>
-      <c r="C25" s="153"/>
+        <v>14</v>
+      </c>
+      <c r="B25" s="153"/>
+      <c r="C25" s="154"/>
       <c r="D25" s="144"/>
       <c r="E25" s="145"/>
       <c r="F25" s="144"/>
       <c r="G25" s="145"/>
-      <c r="H25" s="54"/>
+      <c r="H25" s="54" t="s">
+        <v>43</v>
+      </c>
       <c r="I25" s="54"/>
       <c r="J25" s="50"/>
       <c r="K25" s="138"/>
@@ -3301,14 +3354,14 @@
       <c r="A26" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="152"/>
-      <c r="C26" s="153"/>
+      <c r="B26" s="153"/>
+      <c r="C26" s="154"/>
       <c r="D26" s="144"/>
       <c r="E26" s="145"/>
       <c r="F26" s="144"/>
       <c r="G26" s="145"/>
       <c r="H26" s="62" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I26" s="62"/>
       <c r="J26" s="62"/>
@@ -3318,112 +3371,128 @@
       <c r="A27" s="55">
         <v>922</v>
       </c>
-      <c r="B27" s="154"/>
-      <c r="C27" s="155"/>
+      <c r="B27" s="155"/>
+      <c r="C27" s="156"/>
       <c r="D27" s="146"/>
       <c r="E27" s="147"/>
       <c r="F27" s="146"/>
       <c r="G27" s="147"/>
-      <c r="H27" s="54"/>
+      <c r="H27" s="54" t="s">
+        <v>42</v>
+      </c>
       <c r="I27" s="54"/>
       <c r="J27" s="50"/>
       <c r="K27" s="139"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" s="132" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C28" s="133"/>
       <c r="D28" s="132" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E28" s="133"/>
       <c r="F28" s="132" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G28" s="133"/>
       <c r="H28" s="130" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I28" s="130"/>
       <c r="J28" s="47" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K28" s="63" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
       <c r="A29" s="50">
         <v>4</v>
       </c>
-      <c r="B29" s="150"/>
-      <c r="C29" s="151"/>
-      <c r="D29" s="142"/>
+      <c r="B29" s="151" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="152"/>
+      <c r="D29" s="142" t="s">
+        <v>49</v>
+      </c>
       <c r="E29" s="143"/>
-      <c r="F29" s="142"/>
+      <c r="F29" s="142" t="s">
+        <v>47</v>
+      </c>
       <c r="G29" s="143"/>
-      <c r="H29" s="148" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="149"/>
-      <c r="J29" s="57"/>
+      <c r="H29" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="158"/>
+      <c r="J29" s="57" t="s">
+        <v>55</v>
+      </c>
       <c r="K29" s="137"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="152"/>
-      <c r="C30" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B30" s="153"/>
+      <c r="C30" s="154"/>
       <c r="D30" s="144"/>
       <c r="E30" s="145"/>
       <c r="F30" s="144"/>
       <c r="G30" s="145"/>
       <c r="H30" s="47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I30" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J30" s="47" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K30" s="138"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="152"/>
-      <c r="C31" s="153"/>
+        <v>7</v>
+      </c>
+      <c r="B31" s="153"/>
+      <c r="C31" s="154"/>
       <c r="D31" s="144"/>
       <c r="E31" s="145"/>
       <c r="F31" s="144"/>
       <c r="G31" s="145"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="50"/>
+      <c r="H31" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="K31" s="138"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="152"/>
-      <c r="C32" s="153"/>
+      <c r="B32" s="153"/>
+      <c r="C32" s="154"/>
       <c r="D32" s="144"/>
       <c r="E32" s="145"/>
       <c r="F32" s="144"/>
       <c r="G32" s="145"/>
       <c r="H32" s="47" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I32" s="47" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J32" s="47"/>
       <c r="K32" s="138"/>
@@ -3432,110 +3501,130 @@
       <c r="A33" s="55">
         <v>823</v>
       </c>
-      <c r="B33" s="154"/>
-      <c r="C33" s="155"/>
+      <c r="B33" s="155"/>
+      <c r="C33" s="156"/>
       <c r="D33" s="146"/>
       <c r="E33" s="147"/>
       <c r="F33" s="146"/>
       <c r="G33" s="147"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
+      <c r="H33" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>2</v>
+      </c>
       <c r="J33" s="50"/>
       <c r="K33" s="139"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B34" s="132" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C34" s="133"/>
       <c r="D34" s="132" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E34" s="133"/>
       <c r="F34" s="132" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G34" s="133"/>
       <c r="H34" s="130" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I34" s="130"/>
       <c r="J34" s="47" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K34" s="63" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="50">
         <v>5</v>
       </c>
-      <c r="B35" s="150"/>
-      <c r="C35" s="151"/>
-      <c r="D35" s="142"/>
+      <c r="B35" s="151" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="152"/>
+      <c r="D35" s="142" t="s">
+        <v>49</v>
+      </c>
       <c r="E35" s="143"/>
-      <c r="F35" s="142"/>
+      <c r="F35" s="142" t="s">
+        <v>47</v>
+      </c>
       <c r="G35" s="143"/>
-      <c r="H35" s="148"/>
-      <c r="I35" s="149"/>
-      <c r="J35" s="57"/>
+      <c r="H35" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="158"/>
+      <c r="J35" s="57" t="s">
+        <v>55</v>
+      </c>
       <c r="K35" s="137"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="152"/>
-      <c r="C36" s="153"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="153"/>
+      <c r="C36" s="154"/>
       <c r="D36" s="144"/>
       <c r="E36" s="145"/>
       <c r="F36" s="144"/>
       <c r="G36" s="145"/>
       <c r="H36" s="47" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I36" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J36" s="47" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K36" s="138"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="152"/>
-      <c r="C37" s="153"/>
+        <v>7</v>
+      </c>
+      <c r="B37" s="153"/>
+      <c r="C37" s="154"/>
       <c r="D37" s="144"/>
       <c r="E37" s="145"/>
       <c r="F37" s="144"/>
       <c r="G37" s="145"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="50"/>
+      <c r="H37" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="J37" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="K37" s="138"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="152"/>
-      <c r="C38" s="153"/>
+      <c r="B38" s="153"/>
+      <c r="C38" s="154"/>
       <c r="D38" s="144"/>
       <c r="E38" s="145"/>
       <c r="F38" s="144"/>
       <c r="G38" s="145"/>
       <c r="H38" s="47" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I38" s="47" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J38" s="47"/>
       <c r="K38" s="138"/>
@@ -3544,14 +3633,18 @@
       <c r="A39" s="55">
         <v>823</v>
       </c>
-      <c r="B39" s="154"/>
-      <c r="C39" s="155"/>
+      <c r="B39" s="155"/>
+      <c r="C39" s="156"/>
       <c r="D39" s="146"/>
       <c r="E39" s="147"/>
       <c r="F39" s="146"/>
       <c r="G39" s="147"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
+      <c r="H39" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="54" t="s">
+        <v>2</v>
+      </c>
       <c r="J39" s="50"/>
       <c r="K39" s="139"/>
     </row>
@@ -3956,15 +4049,17 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H34:I34"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C13"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B29:C33"/>
     <mergeCell ref="B35:C39"/>
     <mergeCell ref="D29:E33"/>
     <mergeCell ref="D35:E39"/>
@@ -3973,19 +4068,17 @@
     <mergeCell ref="D9:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="F29:G33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B21:K21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="B23:C27"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D15:E19"/>
     <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H8:I8"/>

</xml_diff>

<commit_message>
Chỉnh sửa file Testcase
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\OneDrive - Hanoi University of Science and Technology\BaiGiang\Quantriduan\DemoTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\National Brother\Documents\GitHub\Qu-n-l-d-n-CNTT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{C2329458-F936-4E58-B5C2-98927AEFA968}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{DA92033F-E7E2-40F0-97C5-4B82ECF31751}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="16" r:id="rId1"/>
@@ -20,17 +19,17 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyen Duc Tien</author>
   </authors>
   <commentList>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="H22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="J22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="A23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="H24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="I24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="J24" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="A25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -156,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="H26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="I26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -182,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="A27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>Online ID</t>
   </si>
@@ -208,12 +207,6 @@
     <t>Resp</t>
   </si>
   <si>
-    <t>23/08/2008</t>
-  </si>
-  <si>
-    <t>BUG21312</t>
-  </si>
-  <si>
     <t>Subtopic(abnormality)</t>
   </si>
   <si>
@@ -316,24 +309,12 @@
     <t>Not OK</t>
   </si>
   <si>
-    <t>TienND</t>
-  </si>
-  <si>
     <t>Test Date</t>
   </si>
   <si>
     <t>Repairer</t>
   </si>
   <si>
-    <t>AnhDV</t>
-  </si>
-  <si>
-    <t>20/08/2008</t>
-  </si>
-  <si>
-    <t>DinhPX</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
@@ -343,37 +324,6 @@
     <t>Related Software:</t>
   </si>
   <si>
-    <t>Xem được phim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Mpeg
-</t>
-  </si>
-  <si>
-    <t>1. Add film mpeg
-2. Mo VLC
-3. Gõ địa chỉ 192.168.0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Không có tham số dòng lệnh
-</t>
-  </si>
-  <si>
-    <t>1. Gõ duy nhất tên chương trình, không có tham số dòng lệnh</t>
-  </si>
-  <si>
-    <t>Chạy được</t>
-  </si>
-  <si>
-    <t>Không có tham số dòng lệnh, nhưng nhập từ Task Manager</t>
-  </si>
-  <si>
-    <t>File Mpeg có thời lượng 3s</t>
-  </si>
-  <si>
-    <t>BUG213</t>
-  </si>
-  <si>
     <t>Tested and result is correct</t>
   </si>
   <si>
@@ -422,13 +372,13 @@
     <t>ID Fmt:</t>
   </si>
   <si>
-    <t>Hear and Note</t>
+    <t>Quản lý bệnh án</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
@@ -1238,95 +1188,95 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1505,23 +1455,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1557,23 +1490,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1749,14 +1665,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <tabColor indexed="46"/>
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -1801,7 +1717,7 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -1883,7 +1799,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="O6" s="127" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P6" s="127"/>
       <c r="Q6" s="127"/>
@@ -1917,10 +1833,10 @@
       <c r="B9" s="30"/>
       <c r="C9" s="18"/>
       <c r="D9" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -1931,9 +1847,11 @@
       <c r="B10" s="30"/>
       <c r="C10" s="18"/>
       <c r="D10" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="28"/>
+        <v>16</v>
+      </c>
+      <c r="E10" s="28">
+        <v>1</v>
+      </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="82"/>
@@ -1941,7 +1859,7 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="124" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
@@ -1955,34 +1873,33 @@
       <c r="B11" s="30"/>
       <c r="C11" s="18"/>
       <c r="D11" s="31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E11" s="128">
-        <f ca="1">TODAY()</f>
-        <v>43206</v>
+        <v>43831</v>
       </c>
       <c r="F11" s="128"/>
       <c r="G11" s="128"/>
       <c r="H11" s="82"/>
       <c r="L11" s="33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="V11" s="33"/>
       <c r="X11" s="19"/>
@@ -1990,7 +1907,7 @@
     <row r="12" spans="1:24">
       <c r="B12" s="30"/>
       <c r="L12" s="34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
@@ -2068,7 +1985,7 @@
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E15" s="81"/>
       <c r="F15" s="81"/>
@@ -2199,7 +2116,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
       <c r="L19" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
@@ -2251,7 +2168,7 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E22" s="81"/>
       <c r="F22" s="81"/>
@@ -2278,7 +2195,7 @@
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="L24" s="124" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="M24" s="114"/>
       <c r="N24" s="114"/>
@@ -2413,7 +2330,7 @@
     <row r="31" spans="2:35">
       <c r="B31" s="15"/>
       <c r="C31" s="39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="28"/>
@@ -2449,7 +2366,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2519,7 +2436,7 @@
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
       <c r="C34" s="39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -2555,7 +2472,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2816,14 +2733,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2837,37 +2754,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="65" customFormat="1">
       <c r="A1" s="87" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B1" s="88" t="str">
         <f>Overview!E9</f>
-        <v>Hear and Note</v>
+        <v>Quản lý bệnh án</v>
       </c>
       <c r="C1" s="88"/>
       <c r="D1" s="88"/>
       <c r="E1" s="89"/>
       <c r="F1" s="89"/>
       <c r="G1" s="90" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H1" s="91" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J1" s="92" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="K1" s="93"/>
     </row>
     <row r="2" spans="1:11" s="65" customFormat="1">
       <c r="A2" s="126" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="95"/>
@@ -2875,23 +2792,23 @@
       <c r="F2" s="96"/>
       <c r="G2" s="97"/>
       <c r="H2" s="98" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="I2" s="112">
         <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
       <c r="A3" s="94" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C3" s="95"/>
       <c r="D3" s="95"/>
@@ -2899,14 +2816,14 @@
       <c r="F3" s="96"/>
       <c r="G3" s="97"/>
       <c r="H3" s="98" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="I3" s="113">
         <f>COUNTIF(H2:H787,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="99" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="K3" s="100"/>
     </row>
@@ -2918,7 +2835,7 @@
       <c r="E4" s="96"/>
       <c r="F4" s="96"/>
       <c r="G4" s="102" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="H4" s="95"/>
       <c r="I4" s="112">
@@ -2956,336 +2873,304 @@
     </row>
     <row r="7" spans="1:11" ht="10.5" customHeight="1">
       <c r="A7" s="109" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="129" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="129"/>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
+        <v>8</v>
+      </c>
+      <c r="B7" s="156" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="156"/>
+      <c r="I7" s="156"/>
+      <c r="J7" s="156"/>
+      <c r="K7" s="156"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="130"/>
+      <c r="D8" s="129" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="130"/>
+      <c r="F8" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="132" t="s">
+      <c r="G8" s="130"/>
+      <c r="H8" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="133"/>
-      <c r="D8" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="133"/>
-      <c r="F8" s="132" t="s">
+      <c r="I8" s="157"/>
+      <c r="J8" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="133"/>
-      <c r="H8" s="131" t="s">
+      <c r="K8" s="49" t="s">
         <v>31</v>
-      </c>
-      <c r="I8" s="131"/>
-      <c r="J8" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="49" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="151" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="152"/>
-      <c r="D9" s="142" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="143"/>
-      <c r="F9" s="51" t="s">
-        <v>52</v>
-      </c>
+      <c r="B9" s="132"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="51"/>
       <c r="G9" s="66"/>
-      <c r="H9" s="140" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="141"/>
+      <c r="H9" s="147"/>
+      <c r="I9" s="148"/>
       <c r="J9" s="50"/>
-      <c r="K9" s="137"/>
+      <c r="K9" s="151"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="153"/>
-      <c r="C10" s="154"/>
-      <c r="D10" s="144"/>
-      <c r="E10" s="145"/>
+        <v>32</v>
+      </c>
+      <c r="B10" s="134"/>
+      <c r="C10" s="135"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="144"/>
       <c r="F10" s="52"/>
       <c r="G10" s="67"/>
       <c r="H10" s="47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="138"/>
+        <v>37</v>
+      </c>
+      <c r="K10" s="152"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="153"/>
-      <c r="C11" s="154"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="145"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="134"/>
+      <c r="C11" s="135"/>
+      <c r="D11" s="143"/>
+      <c r="E11" s="144"/>
       <c r="F11" s="52"/>
       <c r="G11" s="67"/>
-      <c r="H11" s="54" t="s">
-        <v>43</v>
-      </c>
+      <c r="H11" s="54"/>
       <c r="I11" s="54"/>
       <c r="J11" s="50"/>
-      <c r="K11" s="138"/>
+      <c r="K11" s="152"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="153"/>
-      <c r="C12" s="154"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="145"/>
+      <c r="B12" s="134"/>
+      <c r="C12" s="135"/>
+      <c r="D12" s="143"/>
+      <c r="E12" s="144"/>
       <c r="F12" s="52"/>
       <c r="G12" s="67"/>
       <c r="H12" s="47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J12" s="47"/>
-      <c r="K12" s="138"/>
+      <c r="K12" s="152"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="55">
         <v>981</v>
       </c>
-      <c r="B13" s="155"/>
-      <c r="C13" s="156"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="147"/>
+      <c r="B13" s="136"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="145"/>
+      <c r="E13" s="146"/>
       <c r="F13" s="56"/>
       <c r="G13" s="68"/>
-      <c r="H13" s="58" t="s">
-        <v>42</v>
-      </c>
+      <c r="H13" s="58"/>
       <c r="I13" s="58"/>
       <c r="J13" s="59"/>
-      <c r="K13" s="139"/>
+      <c r="K13" s="153"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="139" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="140"/>
+      <c r="D14" s="139" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="140"/>
+      <c r="F14" s="139" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="135" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="136"/>
-      <c r="D14" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="136"/>
-      <c r="F14" s="135" t="s">
+      <c r="G14" s="140"/>
+      <c r="H14" s="138" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="138"/>
+      <c r="J14" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="136"/>
-      <c r="H14" s="150" t="s">
+      <c r="K14" s="61" t="s">
         <v>31</v>
-      </c>
-      <c r="I14" s="150"/>
-      <c r="J14" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="61" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="10.5" customHeight="1">
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="151" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="152"/>
-      <c r="D15" s="142" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="143"/>
-      <c r="F15" s="51" t="s">
-        <v>52</v>
-      </c>
+      <c r="B15" s="132"/>
+      <c r="C15" s="133"/>
+      <c r="D15" s="141"/>
+      <c r="E15" s="142"/>
+      <c r="F15" s="51"/>
       <c r="G15" s="66"/>
-      <c r="H15" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I15" s="158"/>
-      <c r="J15" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="137"/>
+      <c r="H15" s="149"/>
+      <c r="I15" s="150"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="151"/>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="145"/>
+        <v>32</v>
+      </c>
+      <c r="B16" s="134"/>
+      <c r="C16" s="135"/>
+      <c r="D16" s="143"/>
+      <c r="E16" s="144"/>
       <c r="F16" s="52"/>
       <c r="G16" s="67"/>
       <c r="H16" s="62" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I16" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" s="138"/>
+        <v>37</v>
+      </c>
+      <c r="K16" s="152"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="153"/>
-      <c r="C17" s="154"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="145"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="134"/>
+      <c r="C17" s="135"/>
+      <c r="D17" s="143"/>
+      <c r="E17" s="144"/>
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
-      <c r="H17" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" s="138"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="152"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="153"/>
-      <c r="C18" s="154"/>
-      <c r="D18" s="144"/>
-      <c r="E18" s="145"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="135"/>
+      <c r="D18" s="143"/>
+      <c r="E18" s="144"/>
       <c r="F18" s="52"/>
       <c r="G18" s="67"/>
       <c r="H18" s="62" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J18" s="62"/>
-      <c r="K18" s="138"/>
+      <c r="K18" s="152"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="55">
         <v>921</v>
       </c>
-      <c r="B19" s="155"/>
-      <c r="C19" s="156"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="147"/>
+      <c r="B19" s="136"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="145"/>
+      <c r="E19" s="146"/>
       <c r="F19" s="56"/>
       <c r="G19" s="68"/>
-      <c r="H19" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="54" t="s">
-        <v>2</v>
-      </c>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
       <c r="J19" s="50"/>
-      <c r="K19" s="138"/>
+      <c r="K19" s="152"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="109" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="134" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="134"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="129"/>
-      <c r="H20" s="129"/>
-      <c r="I20" s="129"/>
-      <c r="J20" s="129"/>
-      <c r="K20" s="129"/>
+        <v>9</v>
+      </c>
+      <c r="B20" s="158" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="158"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="156"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="156"/>
+      <c r="J20" s="156"/>
+      <c r="K20" s="156"/>
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
       <c r="A21" s="110" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="148" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="148"/>
-      <c r="D21" s="149"/>
-      <c r="E21" s="149"/>
-      <c r="F21" s="149"/>
-      <c r="G21" s="149"/>
-      <c r="H21" s="149"/>
-      <c r="I21" s="149"/>
-      <c r="J21" s="149"/>
-      <c r="K21" s="149"/>
+        <v>7</v>
+      </c>
+      <c r="B21" s="154" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="154"/>
+      <c r="D21" s="155"/>
+      <c r="E21" s="155"/>
+      <c r="F21" s="155"/>
+      <c r="G21" s="155"/>
+      <c r="H21" s="155"/>
+      <c r="I21" s="155"/>
+      <c r="J21" s="155"/>
+      <c r="K21" s="155"/>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A22" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="139" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="140"/>
+      <c r="D22" s="139" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="140"/>
+      <c r="F22" s="139" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="135" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="136"/>
-      <c r="D22" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="136"/>
-      <c r="F22" s="135" t="s">
+      <c r="G22" s="140"/>
+      <c r="H22" s="138" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="138"/>
+      <c r="J22" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="136"/>
-      <c r="H22" s="150" t="s">
+      <c r="K22" s="62" t="s">
         <v>31</v>
-      </c>
-      <c r="I22" s="150"/>
-      <c r="J22" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="62" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
@@ -3293,360 +3178,308 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B23" s="151" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="152"/>
-      <c r="D23" s="142" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="143"/>
-      <c r="F23" s="142" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="143"/>
-      <c r="H23" s="140" t="s">
-        <v>37</v>
-      </c>
-      <c r="I23" s="141"/>
+      <c r="B23" s="132"/>
+      <c r="C23" s="133"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="141"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="147"/>
+      <c r="I23" s="148"/>
       <c r="J23" s="50"/>
-      <c r="K23" s="137"/>
+      <c r="K23" s="151"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="134"/>
+      <c r="C24" s="135"/>
+      <c r="D24" s="143"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="144"/>
+      <c r="H24" s="62" t="s">
         <v>34</v>
-      </c>
-      <c r="B24" s="153"/>
-      <c r="C24" s="154"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="145"/>
-      <c r="H24" s="62" t="s">
-        <v>36</v>
       </c>
       <c r="I24" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="K24" s="138"/>
+        <v>37</v>
+      </c>
+      <c r="K24" s="152"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="153"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="54" t="s">
-        <v>43</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B25" s="134"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="143"/>
+      <c r="E25" s="144"/>
+      <c r="F25" s="143"/>
+      <c r="G25" s="144"/>
+      <c r="H25" s="54"/>
       <c r="I25" s="54"/>
       <c r="J25" s="50"/>
-      <c r="K25" s="138"/>
+      <c r="K25" s="152"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="153"/>
-      <c r="C26" s="154"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="145"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="143"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="143"/>
+      <c r="G26" s="144"/>
       <c r="H26" s="62" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I26" s="62"/>
       <c r="J26" s="62"/>
-      <c r="K26" s="138"/>
+      <c r="K26" s="152"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="55">
         <v>922</v>
       </c>
-      <c r="B27" s="155"/>
-      <c r="C27" s="156"/>
-      <c r="D27" s="146"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="146"/>
-      <c r="G27" s="147"/>
-      <c r="H27" s="54" t="s">
-        <v>42</v>
-      </c>
+      <c r="B27" s="136"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="146"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="54"/>
       <c r="I27" s="54"/>
       <c r="J27" s="50"/>
-      <c r="K27" s="139"/>
+      <c r="K27" s="153"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="130"/>
+      <c r="D28" s="129" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="130"/>
+      <c r="F28" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="132" t="s">
+      <c r="G28" s="130"/>
+      <c r="H28" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="133"/>
-      <c r="D28" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="133"/>
-      <c r="F28" s="132" t="s">
+      <c r="I28" s="131"/>
+      <c r="J28" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="133"/>
-      <c r="H28" s="130" t="s">
+      <c r="K28" s="63" t="s">
         <v>31</v>
-      </c>
-      <c r="I28" s="130"/>
-      <c r="J28" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="63" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
       <c r="A29" s="50">
         <v>4</v>
       </c>
-      <c r="B29" s="151" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="152"/>
-      <c r="D29" s="142" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="143"/>
-      <c r="F29" s="142" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="143"/>
-      <c r="H29" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I29" s="158"/>
-      <c r="J29" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="K29" s="137"/>
+      <c r="B29" s="132"/>
+      <c r="C29" s="133"/>
+      <c r="D29" s="141"/>
+      <c r="E29" s="142"/>
+      <c r="F29" s="141"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="149"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="57"/>
+      <c r="K29" s="151"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="134"/>
+      <c r="C30" s="135"/>
+      <c r="D30" s="143"/>
+      <c r="E30" s="144"/>
+      <c r="F30" s="143"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="47" t="s">
         <v>34</v>
-      </c>
-      <c r="B30" s="153"/>
-      <c r="C30" s="154"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="145"/>
-      <c r="H30" s="47" t="s">
-        <v>36</v>
       </c>
       <c r="I30" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J30" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" s="138"/>
+        <v>37</v>
+      </c>
+      <c r="K30" s="152"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="153"/>
-      <c r="C31" s="154"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J31" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="138"/>
+        <v>5</v>
+      </c>
+      <c r="B31" s="134"/>
+      <c r="C31" s="135"/>
+      <c r="D31" s="143"/>
+      <c r="E31" s="144"/>
+      <c r="F31" s="143"/>
+      <c r="G31" s="144"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="152"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="153"/>
-      <c r="C32" s="154"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="145"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="145"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="135"/>
+      <c r="D32" s="143"/>
+      <c r="E32" s="144"/>
+      <c r="F32" s="143"/>
+      <c r="G32" s="144"/>
       <c r="H32" s="47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I32" s="47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J32" s="47"/>
-      <c r="K32" s="138"/>
+      <c r="K32" s="152"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
       <c r="A33" s="55">
         <v>823</v>
       </c>
-      <c r="B33" s="155"/>
-      <c r="C33" s="156"/>
-      <c r="D33" s="146"/>
-      <c r="E33" s="147"/>
-      <c r="F33" s="146"/>
-      <c r="G33" s="147"/>
-      <c r="H33" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I33" s="54" t="s">
-        <v>2</v>
-      </c>
+      <c r="B33" s="136"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="145"/>
+      <c r="E33" s="146"/>
+      <c r="F33" s="145"/>
+      <c r="G33" s="146"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
       <c r="J33" s="50"/>
-      <c r="K33" s="139"/>
+      <c r="K33" s="153"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="130"/>
+      <c r="D34" s="129" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="130"/>
+      <c r="F34" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="132" t="s">
+      <c r="G34" s="130"/>
+      <c r="H34" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="133"/>
-      <c r="D34" s="132" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="133"/>
-      <c r="F34" s="132" t="s">
+      <c r="I34" s="131"/>
+      <c r="J34" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="G34" s="133"/>
-      <c r="H34" s="130" t="s">
+      <c r="K34" s="63" t="s">
         <v>31</v>
-      </c>
-      <c r="I34" s="130"/>
-      <c r="J34" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="K34" s="63" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="50">
         <v>5</v>
       </c>
-      <c r="B35" s="151" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="152"/>
-      <c r="D35" s="142" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="143"/>
-      <c r="F35" s="142" t="s">
-        <v>47</v>
-      </c>
-      <c r="G35" s="143"/>
-      <c r="H35" s="157" t="s">
-        <v>37</v>
-      </c>
-      <c r="I35" s="158"/>
-      <c r="J35" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="K35" s="137"/>
+      <c r="B35" s="132"/>
+      <c r="C35" s="133"/>
+      <c r="D35" s="141"/>
+      <c r="E35" s="142"/>
+      <c r="F35" s="141"/>
+      <c r="G35" s="142"/>
+      <c r="H35" s="149"/>
+      <c r="I35" s="150"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="151"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="134"/>
+      <c r="C36" s="135"/>
+      <c r="D36" s="143"/>
+      <c r="E36" s="144"/>
+      <c r="F36" s="143"/>
+      <c r="G36" s="144"/>
+      <c r="H36" s="47" t="s">
         <v>34</v>
-      </c>
-      <c r="B36" s="153"/>
-      <c r="C36" s="154"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="47" t="s">
-        <v>36</v>
       </c>
       <c r="I36" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J36" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="138"/>
+        <v>37</v>
+      </c>
+      <c r="K36" s="152"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="153"/>
-      <c r="C37" s="154"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="K37" s="138"/>
+        <v>5</v>
+      </c>
+      <c r="B37" s="134"/>
+      <c r="C37" s="135"/>
+      <c r="D37" s="143"/>
+      <c r="E37" s="144"/>
+      <c r="F37" s="143"/>
+      <c r="G37" s="144"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="152"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="153"/>
-      <c r="C38" s="154"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="145"/>
-      <c r="F38" s="144"/>
-      <c r="G38" s="145"/>
+      <c r="B38" s="134"/>
+      <c r="C38" s="135"/>
+      <c r="D38" s="143"/>
+      <c r="E38" s="144"/>
+      <c r="F38" s="143"/>
+      <c r="G38" s="144"/>
       <c r="H38" s="47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I38" s="47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J38" s="47"/>
-      <c r="K38" s="138"/>
+      <c r="K38" s="152"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="55">
         <v>823</v>
       </c>
-      <c r="B39" s="155"/>
-      <c r="C39" s="156"/>
-      <c r="D39" s="146"/>
-      <c r="E39" s="147"/>
-      <c r="F39" s="146"/>
-      <c r="G39" s="147"/>
-      <c r="H39" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="I39" s="54" t="s">
-        <v>2</v>
-      </c>
+      <c r="B39" s="136"/>
+      <c r="C39" s="137"/>
+      <c r="D39" s="145"/>
+      <c r="E39" s="146"/>
+      <c r="F39" s="145"/>
+      <c r="G39" s="146"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
       <c r="J39" s="50"/>
-      <c r="K39" s="139"/>
+      <c r="K39" s="153"/>
     </row>
     <row r="40" spans="1:11" s="65" customFormat="1">
       <c r="A40" s="72"/>
@@ -4049,36 +3882,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="B35:C39"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="D35:E39"/>
-    <mergeCell ref="F35:G39"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C27"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="B15:C19"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H8:I8"/>
@@ -4095,6 +3898,36 @@
     <mergeCell ref="D23:E27"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="F23:G27"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="F29:G33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="B35:C39"/>
+    <mergeCell ref="D29:E33"/>
+    <mergeCell ref="D35:E39"/>
+    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C27"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B29:C33"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H35:I35">

</xml_diff>

<commit_message>
Kiểm tra thông số của các biểu mẫu
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
   <si>
     <t>Online ID</t>
   </si>
@@ -388,6 +388,24 @@
   </si>
   <si>
     <t>HuyBK</t>
+  </si>
+  <si>
+    <t>Test các biểu mẫu bệnh án</t>
+  </si>
+  <si>
+    <t>Kiểm tra thông tin các thông số trong bảng bệnh án</t>
+  </si>
+  <si>
+    <t>Hoàn Thành</t>
+  </si>
+  <si>
+    <t>BUG13213</t>
+  </si>
+  <si>
+    <t>HungND</t>
+  </si>
+  <si>
+    <t>Biểu mẫu số 3: Thông số không đúng yêu cầu vẫn có thể  gửi.</t>
   </si>
 </sst>
 </file>
@@ -2754,8 +2772,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2811,7 +2829,7 @@
       </c>
       <c r="I2" s="112">
         <f>COUNTIF(H2:H787,"Not OK")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="99" t="s">
         <v>42</v>
@@ -3062,16 +3080,28 @@
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="150"/>
+      <c r="B15" s="150" t="s">
+        <v>63</v>
+      </c>
       <c r="C15" s="151"/>
-      <c r="D15" s="142"/>
+      <c r="D15" s="142" t="s">
+        <v>64</v>
+      </c>
       <c r="E15" s="143"/>
-      <c r="F15" s="51"/>
+      <c r="F15" s="51" t="s">
+        <v>65</v>
+      </c>
       <c r="G15" s="66"/>
-      <c r="H15" s="148"/>
+      <c r="H15" s="148" t="s">
+        <v>35</v>
+      </c>
       <c r="I15" s="149"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="137"/>
+      <c r="J15" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="137" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="62" t="s">
@@ -3104,9 +3134,15 @@
       <c r="E17" s="145"/>
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="50"/>
+      <c r="H17" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="50" t="s">
+        <v>67</v>
+      </c>
       <c r="K17" s="138"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
@@ -3138,8 +3174,12 @@
       <c r="E19" s="147"/>
       <c r="F19" s="56"/>
       <c r="G19" s="68"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
+      <c r="H19" s="54">
+        <v>43813</v>
+      </c>
+      <c r="I19" s="54">
+        <v>43814</v>
+      </c>
       <c r="J19" s="50"/>
       <c r="K19" s="138"/>
     </row>

</xml_diff>

<commit_message>
Test giao diện thông tin bệnh nhân
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
   <si>
     <t>Online ID</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>Biểu mẫu số 3: Thông số không đúng yêu cầu vẫn có thể  gửi.</t>
+  </si>
+  <si>
+    <t>Check bảng thông tin bệnh nhân</t>
+  </si>
+  <si>
+    <t>Kiểm tra các trường thông tin về bệnh nhân</t>
   </si>
 </sst>
 </file>
@@ -1221,95 +1227,95 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2773,7 +2779,7 @@
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:K19"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2805,7 +2811,7 @@
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J1" s="92" t="s">
         <v>41</v>
@@ -2908,39 +2914,39 @@
       <c r="A7" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="129" t="s">
+      <c r="B7" s="156" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="129"/>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="156"/>
+      <c r="I7" s="156"/>
+      <c r="J7" s="156"/>
+      <c r="K7" s="156"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="133"/>
-      <c r="D8" s="132" t="s">
+      <c r="C8" s="130"/>
+      <c r="D8" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="133"/>
-      <c r="F8" s="132" t="s">
+      <c r="E8" s="130"/>
+      <c r="F8" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="133"/>
-      <c r="H8" s="131" t="s">
+      <c r="G8" s="130"/>
+      <c r="H8" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="131"/>
+      <c r="I8" s="157"/>
       <c r="J8" s="48" t="s">
         <v>30</v>
       </c>
@@ -2952,33 +2958,33 @@
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="150" t="s">
+      <c r="B9" s="131" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="151"/>
-      <c r="D9" s="142" t="s">
+      <c r="C9" s="132"/>
+      <c r="D9" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="143"/>
+      <c r="E9" s="141"/>
       <c r="F9" s="51" t="s">
         <v>60</v>
       </c>
       <c r="G9" s="66"/>
-      <c r="H9" s="140" t="s">
+      <c r="H9" s="146" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="141"/>
+      <c r="I9" s="147"/>
       <c r="J9" s="50"/>
-      <c r="K9" s="137"/>
+      <c r="K9" s="153"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="152"/>
-      <c r="C10" s="153"/>
-      <c r="D10" s="144"/>
-      <c r="E10" s="145"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="134"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="143"/>
       <c r="F10" s="52"/>
       <c r="G10" s="67"/>
       <c r="H10" s="47" t="s">
@@ -2990,16 +2996,16 @@
       <c r="J10" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="138"/>
+      <c r="K10" s="154"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="152"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="145"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="142"/>
+      <c r="E11" s="143"/>
       <c r="F11" s="52"/>
       <c r="G11" s="67"/>
       <c r="H11" s="54" t="s">
@@ -3009,16 +3015,16 @@
         <v>62</v>
       </c>
       <c r="J11" s="50"/>
-      <c r="K11" s="138"/>
+      <c r="K11" s="154"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="152"/>
-      <c r="C12" s="153"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="145"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="142"/>
+      <c r="E12" s="143"/>
       <c r="F12" s="52"/>
       <c r="G12" s="67"/>
       <c r="H12" s="47" t="s">
@@ -3028,16 +3034,16 @@
         <v>33</v>
       </c>
       <c r="J12" s="47"/>
-      <c r="K12" s="138"/>
+      <c r="K12" s="154"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="55">
         <v>981</v>
       </c>
-      <c r="B13" s="154"/>
-      <c r="C13" s="155"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="147"/>
+      <c r="B13" s="135"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="145"/>
       <c r="F13" s="56"/>
       <c r="G13" s="68"/>
       <c r="H13" s="58">
@@ -3047,28 +3053,28 @@
         <v>43814</v>
       </c>
       <c r="J13" s="59"/>
-      <c r="K13" s="139"/>
+      <c r="K13" s="155"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="135" t="s">
+      <c r="B14" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="136"/>
-      <c r="D14" s="135" t="s">
+      <c r="C14" s="139"/>
+      <c r="D14" s="138" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="136"/>
-      <c r="F14" s="135" t="s">
+      <c r="E14" s="139"/>
+      <c r="F14" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="136"/>
-      <c r="H14" s="158" t="s">
+      <c r="G14" s="139"/>
+      <c r="H14" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="158"/>
+      <c r="I14" s="137"/>
       <c r="J14" s="62" t="s">
         <v>30</v>
       </c>
@@ -3080,14 +3086,14 @@
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="150" t="s">
+      <c r="B15" s="131" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="151"/>
-      <c r="D15" s="142" t="s">
+      <c r="C15" s="132"/>
+      <c r="D15" s="140" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="143"/>
+      <c r="E15" s="141"/>
       <c r="F15" s="51" t="s">
         <v>65</v>
       </c>
@@ -3099,7 +3105,7 @@
       <c r="J15" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="137" t="s">
+      <c r="K15" s="153" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3107,10 +3113,10 @@
       <c r="A16" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="152"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="145"/>
+      <c r="B16" s="133"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="143"/>
       <c r="F16" s="52"/>
       <c r="G16" s="67"/>
       <c r="H16" s="62" t="s">
@@ -3122,16 +3128,16 @@
       <c r="J16" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="138"/>
+      <c r="K16" s="154"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="152"/>
-      <c r="C17" s="153"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="145"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="142"/>
+      <c r="E17" s="143"/>
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
       <c r="H17" s="54" t="s">
@@ -3143,16 +3149,16 @@
       <c r="J17" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="138"/>
+      <c r="K17" s="154"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="152"/>
-      <c r="C18" s="153"/>
-      <c r="D18" s="144"/>
-      <c r="E18" s="145"/>
+      <c r="B18" s="133"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="143"/>
       <c r="F18" s="52"/>
       <c r="G18" s="67"/>
       <c r="H18" s="62" t="s">
@@ -3162,16 +3168,16 @@
         <v>33</v>
       </c>
       <c r="J18" s="62"/>
-      <c r="K18" s="138"/>
+      <c r="K18" s="154"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="55">
         <v>921</v>
       </c>
-      <c r="B19" s="154"/>
-      <c r="C19" s="155"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="147"/>
+      <c r="B19" s="135"/>
+      <c r="C19" s="136"/>
+      <c r="D19" s="144"/>
+      <c r="E19" s="145"/>
       <c r="F19" s="56"/>
       <c r="G19" s="68"/>
       <c r="H19" s="54">
@@ -3181,62 +3187,62 @@
         <v>43814</v>
       </c>
       <c r="J19" s="50"/>
-      <c r="K19" s="138"/>
+      <c r="K19" s="154"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="134" t="s">
+      <c r="B20" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="134"/>
-      <c r="D20" s="129"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="129"/>
-      <c r="H20" s="129"/>
-      <c r="I20" s="129"/>
-      <c r="J20" s="129"/>
-      <c r="K20" s="129"/>
+      <c r="C20" s="158"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="156"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="156"/>
+      <c r="J20" s="156"/>
+      <c r="K20" s="156"/>
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
       <c r="A21" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="156" t="s">
+      <c r="B21" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="156"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="157"/>
+      <c r="C21" s="150"/>
+      <c r="D21" s="151"/>
+      <c r="E21" s="151"/>
+      <c r="F21" s="151"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="151"/>
+      <c r="I21" s="151"/>
+      <c r="J21" s="151"/>
+      <c r="K21" s="151"/>
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A22" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="135" t="s">
+      <c r="B22" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="136"/>
-      <c r="D22" s="135" t="s">
+      <c r="C22" s="139"/>
+      <c r="D22" s="138" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="136"/>
-      <c r="F22" s="135" t="s">
+      <c r="E22" s="139"/>
+      <c r="F22" s="138" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="136"/>
-      <c r="H22" s="158" t="s">
+      <c r="G22" s="139"/>
+      <c r="H22" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="158"/>
+      <c r="I22" s="137"/>
       <c r="J22" s="62" t="s">
         <v>30</v>
       </c>
@@ -3249,27 +3255,35 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B23" s="150"/>
-      <c r="C23" s="151"/>
-      <c r="D23" s="142"/>
-      <c r="E23" s="143"/>
-      <c r="F23" s="142"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="140"/>
-      <c r="I23" s="141"/>
+      <c r="B23" s="131" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="132"/>
+      <c r="D23" s="140" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="141"/>
+      <c r="F23" s="140" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="141"/>
+      <c r="H23" s="146" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="147"/>
       <c r="J23" s="50"/>
-      <c r="K23" s="137"/>
+      <c r="K23" s="153"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="152"/>
-      <c r="C24" s="153"/>
-      <c r="D24" s="144"/>
-      <c r="E24" s="145"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="145"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="142"/>
+      <c r="E24" s="143"/>
+      <c r="F24" s="142"/>
+      <c r="G24" s="143"/>
       <c r="H24" s="62" t="s">
         <v>34</v>
       </c>
@@ -3279,75 +3293,83 @@
       <c r="J24" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="138"/>
+      <c r="K24" s="154"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="152"/>
-      <c r="C25" s="153"/>
-      <c r="D25" s="144"/>
-      <c r="E25" s="145"/>
-      <c r="F25" s="144"/>
-      <c r="G25" s="145"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
+      <c r="B25" s="133"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="142"/>
+      <c r="E25" s="143"/>
+      <c r="F25" s="142"/>
+      <c r="G25" s="143"/>
+      <c r="H25" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="54" t="s">
+        <v>62</v>
+      </c>
       <c r="J25" s="50"/>
-      <c r="K25" s="138"/>
+      <c r="K25" s="154"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="152"/>
-      <c r="C26" s="153"/>
-      <c r="D26" s="144"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="144"/>
-      <c r="G26" s="145"/>
+      <c r="B26" s="133"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="143"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="143"/>
       <c r="H26" s="62" t="s">
         <v>36</v>
       </c>
       <c r="I26" s="62"/>
       <c r="J26" s="62"/>
-      <c r="K26" s="138"/>
+      <c r="K26" s="154"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="55">
         <v>922</v>
       </c>
-      <c r="B27" s="154"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="146"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="146"/>
-      <c r="G27" s="147"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="136"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="144"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="54">
+        <v>43813</v>
+      </c>
+      <c r="I27" s="54">
+        <v>43813</v>
+      </c>
       <c r="J27" s="50"/>
-      <c r="K27" s="139"/>
+      <c r="K27" s="155"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="132" t="s">
+      <c r="B28" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="133"/>
-      <c r="D28" s="132" t="s">
+      <c r="C28" s="130"/>
+      <c r="D28" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="133"/>
-      <c r="F28" s="132" t="s">
+      <c r="E28" s="130"/>
+      <c r="F28" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="133"/>
-      <c r="H28" s="130" t="s">
+      <c r="G28" s="130"/>
+      <c r="H28" s="152" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="130"/>
+      <c r="I28" s="152"/>
       <c r="J28" s="47" t="s">
         <v>30</v>
       </c>
@@ -3359,27 +3381,27 @@
       <c r="A29" s="50">
         <v>4</v>
       </c>
-      <c r="B29" s="150"/>
-      <c r="C29" s="151"/>
-      <c r="D29" s="142"/>
-      <c r="E29" s="143"/>
-      <c r="F29" s="142"/>
-      <c r="G29" s="143"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="140"/>
+      <c r="E29" s="141"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="141"/>
       <c r="H29" s="148"/>
       <c r="I29" s="149"/>
       <c r="J29" s="57"/>
-      <c r="K29" s="137"/>
+      <c r="K29" s="153"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="152"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="145"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="145"/>
+      <c r="B30" s="133"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="142"/>
+      <c r="E30" s="143"/>
+      <c r="F30" s="142"/>
+      <c r="G30" s="143"/>
       <c r="H30" s="47" t="s">
         <v>34</v>
       </c>
@@ -3389,33 +3411,33 @@
       <c r="J30" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="138"/>
+      <c r="K30" s="154"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="152"/>
-      <c r="C31" s="153"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="145"/>
+      <c r="B31" s="133"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="142"/>
+      <c r="E31" s="143"/>
+      <c r="F31" s="142"/>
+      <c r="G31" s="143"/>
       <c r="H31" s="54"/>
       <c r="I31" s="54"/>
       <c r="J31" s="50"/>
-      <c r="K31" s="138"/>
+      <c r="K31" s="154"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="152"/>
-      <c r="C32" s="153"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="145"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="145"/>
+      <c r="B32" s="133"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="142"/>
+      <c r="E32" s="143"/>
+      <c r="F32" s="142"/>
+      <c r="G32" s="143"/>
       <c r="H32" s="47" t="s">
         <v>36</v>
       </c>
@@ -3423,43 +3445,43 @@
         <v>33</v>
       </c>
       <c r="J32" s="47"/>
-      <c r="K32" s="138"/>
+      <c r="K32" s="154"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
       <c r="A33" s="55">
         <v>823</v>
       </c>
-      <c r="B33" s="154"/>
-      <c r="C33" s="155"/>
-      <c r="D33" s="146"/>
-      <c r="E33" s="147"/>
-      <c r="F33" s="146"/>
-      <c r="G33" s="147"/>
+      <c r="B33" s="135"/>
+      <c r="C33" s="136"/>
+      <c r="D33" s="144"/>
+      <c r="E33" s="145"/>
+      <c r="F33" s="144"/>
+      <c r="G33" s="145"/>
       <c r="H33" s="54"/>
       <c r="I33" s="54"/>
       <c r="J33" s="50"/>
-      <c r="K33" s="139"/>
+      <c r="K33" s="155"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="132" t="s">
+      <c r="B34" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="133"/>
-      <c r="D34" s="132" t="s">
+      <c r="C34" s="130"/>
+      <c r="D34" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="133"/>
-      <c r="F34" s="132" t="s">
+      <c r="E34" s="130"/>
+      <c r="F34" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="133"/>
-      <c r="H34" s="130" t="s">
+      <c r="G34" s="130"/>
+      <c r="H34" s="152" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="130"/>
+      <c r="I34" s="152"/>
       <c r="J34" s="47" t="s">
         <v>30</v>
       </c>
@@ -3471,27 +3493,27 @@
       <c r="A35" s="50">
         <v>5</v>
       </c>
-      <c r="B35" s="150"/>
-      <c r="C35" s="151"/>
-      <c r="D35" s="142"/>
-      <c r="E35" s="143"/>
-      <c r="F35" s="142"/>
-      <c r="G35" s="143"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="132"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="141"/>
+      <c r="F35" s="140"/>
+      <c r="G35" s="141"/>
       <c r="H35" s="148"/>
       <c r="I35" s="149"/>
       <c r="J35" s="57"/>
-      <c r="K35" s="137"/>
+      <c r="K35" s="153"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="152"/>
-      <c r="C36" s="153"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="145"/>
+      <c r="B36" s="133"/>
+      <c r="C36" s="134"/>
+      <c r="D36" s="142"/>
+      <c r="E36" s="143"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="143"/>
       <c r="H36" s="47" t="s">
         <v>34</v>
       </c>
@@ -3501,33 +3523,33 @@
       <c r="J36" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="138"/>
+      <c r="K36" s="154"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="152"/>
-      <c r="C37" s="153"/>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
+      <c r="B37" s="133"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="142"/>
+      <c r="E37" s="143"/>
+      <c r="F37" s="142"/>
+      <c r="G37" s="143"/>
       <c r="H37" s="54"/>
       <c r="I37" s="54"/>
       <c r="J37" s="50"/>
-      <c r="K37" s="138"/>
+      <c r="K37" s="154"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="152"/>
-      <c r="C38" s="153"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="145"/>
-      <c r="F38" s="144"/>
-      <c r="G38" s="145"/>
+      <c r="B38" s="133"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="142"/>
+      <c r="E38" s="143"/>
+      <c r="F38" s="142"/>
+      <c r="G38" s="143"/>
       <c r="H38" s="47" t="s">
         <v>36</v>
       </c>
@@ -3535,22 +3557,22 @@
         <v>33</v>
       </c>
       <c r="J38" s="47"/>
-      <c r="K38" s="138"/>
+      <c r="K38" s="154"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="55">
         <v>823</v>
       </c>
-      <c r="B39" s="154"/>
-      <c r="C39" s="155"/>
-      <c r="D39" s="146"/>
-      <c r="E39" s="147"/>
-      <c r="F39" s="146"/>
-      <c r="G39" s="147"/>
+      <c r="B39" s="135"/>
+      <c r="C39" s="136"/>
+      <c r="D39" s="144"/>
+      <c r="E39" s="145"/>
+      <c r="F39" s="144"/>
+      <c r="G39" s="145"/>
       <c r="H39" s="54"/>
       <c r="I39" s="54"/>
       <c r="J39" s="50"/>
-      <c r="K39" s="139"/>
+      <c r="K39" s="155"/>
     </row>
     <row r="40" spans="1:11" s="65" customFormat="1">
       <c r="A40" s="72"/>
@@ -3953,36 +3975,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B35:C39"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="D35:E39"/>
-    <mergeCell ref="F35:G39"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C27"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H8:I8"/>
@@ -3999,6 +3991,36 @@
     <mergeCell ref="D23:E27"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="F23:G27"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="F29:G33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B35:C39"/>
+    <mergeCell ref="D29:E33"/>
+    <mergeCell ref="D35:E39"/>
+    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C27"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H35:I35">

</xml_diff>

<commit_message>
Test giao diện thông tin bác sỹ
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
   <si>
     <t>Online ID</t>
   </si>
@@ -412,6 +412,12 @@
   </si>
   <si>
     <t>Kiểm tra các trường thông tin về bệnh nhân</t>
+  </si>
+  <si>
+    <t>Check giao diện thông tin bác sỹ</t>
+  </si>
+  <si>
+    <t>Kiểm tra các trường thông tin về bác sỹ</t>
   </si>
 </sst>
 </file>
@@ -2778,8 +2784,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2811,7 +2817,7 @@
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1" s="92" t="s">
         <v>41</v>
@@ -3381,13 +3387,21 @@
       <c r="A29" s="50">
         <v>4</v>
       </c>
-      <c r="B29" s="131"/>
+      <c r="B29" s="131" t="s">
+        <v>71</v>
+      </c>
       <c r="C29" s="132"/>
-      <c r="D29" s="140"/>
+      <c r="D29" s="140" t="s">
+        <v>72</v>
+      </c>
       <c r="E29" s="141"/>
-      <c r="F29" s="140"/>
+      <c r="F29" s="140" t="s">
+        <v>65</v>
+      </c>
       <c r="G29" s="141"/>
-      <c r="H29" s="148"/>
+      <c r="H29" s="148" t="s">
+        <v>38</v>
+      </c>
       <c r="I29" s="149"/>
       <c r="J29" s="57"/>
       <c r="K29" s="153"/>
@@ -3423,8 +3437,12 @@
       <c r="E31" s="143"/>
       <c r="F31" s="142"/>
       <c r="G31" s="143"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
+      <c r="H31" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" s="54" t="s">
+        <v>62</v>
+      </c>
       <c r="J31" s="50"/>
       <c r="K31" s="154"/>
     </row>
@@ -3457,8 +3475,12 @@
       <c r="E33" s="145"/>
       <c r="F33" s="144"/>
       <c r="G33" s="145"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
+      <c r="H33" s="54">
+        <v>43813</v>
+      </c>
+      <c r="I33" s="54">
+        <v>43814</v>
+      </c>
       <c r="J33" s="50"/>
       <c r="K33" s="155"/>
     </row>

</xml_diff>

<commit_message>
Check lỗi truy vấn
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
   <si>
     <t>Online ID</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>Kiểm tra các trường thông tin về bác sỹ</t>
+  </si>
+  <si>
+    <t>Check lỗi truy cập CSDL</t>
+  </si>
+  <si>
+    <t>Kiểm tra các lỗi như SQL Injection,..</t>
   </si>
 </sst>
 </file>
@@ -2784,8 +2790,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B14" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2817,7 +2823,7 @@
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" s="92" t="s">
         <v>41</v>
@@ -3515,13 +3521,21 @@
       <c r="A35" s="50">
         <v>5</v>
       </c>
-      <c r="B35" s="131"/>
+      <c r="B35" s="131" t="s">
+        <v>73</v>
+      </c>
       <c r="C35" s="132"/>
-      <c r="D35" s="140"/>
+      <c r="D35" s="140" t="s">
+        <v>74</v>
+      </c>
       <c r="E35" s="141"/>
-      <c r="F35" s="140"/>
+      <c r="F35" s="140" t="s">
+        <v>65</v>
+      </c>
       <c r="G35" s="141"/>
-      <c r="H35" s="148"/>
+      <c r="H35" s="148" t="s">
+        <v>38</v>
+      </c>
       <c r="I35" s="149"/>
       <c r="J35" s="57"/>
       <c r="K35" s="153"/>
@@ -3557,8 +3571,12 @@
       <c r="E37" s="143"/>
       <c r="F37" s="142"/>
       <c r="G37" s="143"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
+      <c r="H37" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>62</v>
+      </c>
       <c r="J37" s="50"/>
       <c r="K37" s="154"/>
     </row>
@@ -3591,8 +3609,12 @@
       <c r="E39" s="145"/>
       <c r="F39" s="144"/>
       <c r="G39" s="145"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
+      <c r="H39" s="54">
+        <v>43813</v>
+      </c>
+      <c r="I39" s="54">
+        <v>43814</v>
+      </c>
       <c r="J39" s="50"/>
       <c r="K39" s="155"/>
     </row>

</xml_diff>

<commit_message>
Thêm Related Document & Related Software
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="4785"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="16" r:id="rId1"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
   <si>
     <t>Online ID</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>Kiểm tra các lỗi như SQL Injection,..</t>
+  </si>
+  <si>
+    <t>MySQL, AWS,...</t>
+  </si>
+  <si>
+    <t>Tài liệu môn quản trị dự án - Tiến NĐ</t>
   </si>
 </sst>
 </file>
@@ -1239,12 +1245,75 @@
       <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1265,69 +1334,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1425,6 +1431,48 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>106493</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>148478</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Hình ảnh 3"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="403412" y="224118"/>
+          <a:ext cx="1081405" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1722,8 +1770,8 @@
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -2038,7 +2086,9 @@
       <c r="D15" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="81"/>
+      <c r="E15" s="81" t="s">
+        <v>76</v>
+      </c>
       <c r="F15" s="81"/>
       <c r="G15" s="81"/>
       <c r="H15" s="81"/>
@@ -2221,7 +2271,9 @@
       <c r="D22" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="81"/>
+      <c r="E22" s="81" t="s">
+        <v>75</v>
+      </c>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
       <c r="H22" s="81"/>
@@ -2790,7 +2842,7 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B14" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="B14" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
@@ -2926,39 +2978,39 @@
       <c r="A7" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="156" t="s">
+      <c r="B7" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="156"/>
-      <c r="H7" s="156"/>
-      <c r="I7" s="156"/>
-      <c r="J7" s="156"/>
-      <c r="K7" s="156"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="129"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="129" t="s">
+      <c r="B8" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="130"/>
-      <c r="D8" s="129" t="s">
+      <c r="C8" s="133"/>
+      <c r="D8" s="132" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="129" t="s">
+      <c r="E8" s="133"/>
+      <c r="F8" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="130"/>
-      <c r="H8" s="157" t="s">
+      <c r="G8" s="133"/>
+      <c r="H8" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="157"/>
+      <c r="I8" s="131"/>
       <c r="J8" s="48" t="s">
         <v>30</v>
       </c>
@@ -2970,33 +3022,33 @@
       <c r="A9" s="50">
         <v>1</v>
       </c>
-      <c r="B9" s="131" t="s">
+      <c r="B9" s="152" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="132"/>
-      <c r="D9" s="140" t="s">
+      <c r="C9" s="153"/>
+      <c r="D9" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="141"/>
+      <c r="E9" s="143"/>
       <c r="F9" s="51" t="s">
         <v>60</v>
       </c>
       <c r="G9" s="66"/>
-      <c r="H9" s="146" t="s">
+      <c r="H9" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="147"/>
+      <c r="I9" s="141"/>
       <c r="J9" s="50"/>
-      <c r="K9" s="153"/>
+      <c r="K9" s="137"/>
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="133"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="142"/>
-      <c r="E10" s="143"/>
+      <c r="B10" s="154"/>
+      <c r="C10" s="155"/>
+      <c r="D10" s="144"/>
+      <c r="E10" s="145"/>
       <c r="F10" s="52"/>
       <c r="G10" s="67"/>
       <c r="H10" s="47" t="s">
@@ -3008,16 +3060,16 @@
       <c r="J10" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="154"/>
+      <c r="K10" s="138"/>
     </row>
     <row r="11" spans="1:11" ht="10.5" customHeight="1">
       <c r="A11" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="133"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="142"/>
-      <c r="E11" s="143"/>
+      <c r="B11" s="154"/>
+      <c r="C11" s="155"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="145"/>
       <c r="F11" s="52"/>
       <c r="G11" s="67"/>
       <c r="H11" s="54" t="s">
@@ -3027,16 +3079,16 @@
         <v>62</v>
       </c>
       <c r="J11" s="50"/>
-      <c r="K11" s="154"/>
+      <c r="K11" s="138"/>
     </row>
     <row r="12" spans="1:11" ht="10.5" customHeight="1">
       <c r="A12" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="133"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="142"/>
-      <c r="E12" s="143"/>
+      <c r="B12" s="154"/>
+      <c r="C12" s="155"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="145"/>
       <c r="F12" s="52"/>
       <c r="G12" s="67"/>
       <c r="H12" s="47" t="s">
@@ -3046,16 +3098,16 @@
         <v>33</v>
       </c>
       <c r="J12" s="47"/>
-      <c r="K12" s="154"/>
+      <c r="K12" s="138"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1">
       <c r="A13" s="55">
         <v>981</v>
       </c>
-      <c r="B13" s="135"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="144"/>
-      <c r="E13" s="145"/>
+      <c r="B13" s="156"/>
+      <c r="C13" s="157"/>
+      <c r="D13" s="146"/>
+      <c r="E13" s="147"/>
       <c r="F13" s="56"/>
       <c r="G13" s="68"/>
       <c r="H13" s="58">
@@ -3065,28 +3117,28 @@
         <v>43814</v>
       </c>
       <c r="J13" s="59"/>
-      <c r="K13" s="155"/>
+      <c r="K13" s="139"/>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="139"/>
-      <c r="D14" s="138" t="s">
+      <c r="C14" s="136"/>
+      <c r="D14" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="139"/>
-      <c r="F14" s="138" t="s">
+      <c r="E14" s="136"/>
+      <c r="F14" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="139"/>
-      <c r="H14" s="137" t="s">
+      <c r="G14" s="136"/>
+      <c r="H14" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="137"/>
+      <c r="I14" s="158"/>
       <c r="J14" s="62" t="s">
         <v>30</v>
       </c>
@@ -3098,14 +3150,14 @@
       <c r="A15" s="50">
         <v>2</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="152" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="132"/>
-      <c r="D15" s="140" t="s">
+      <c r="C15" s="153"/>
+      <c r="D15" s="142" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="141"/>
+      <c r="E15" s="143"/>
       <c r="F15" s="51" t="s">
         <v>65</v>
       </c>
@@ -3117,7 +3169,7 @@
       <c r="J15" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="153" t="s">
+      <c r="K15" s="137" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3125,10 +3177,10 @@
       <c r="A16" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="133"/>
-      <c r="C16" s="134"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="143"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="145"/>
       <c r="F16" s="52"/>
       <c r="G16" s="67"/>
       <c r="H16" s="62" t="s">
@@ -3140,16 +3192,16 @@
       <c r="J16" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="154"/>
+      <c r="K16" s="138"/>
     </row>
     <row r="17" spans="1:11" ht="10.5" customHeight="1">
       <c r="A17" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="133"/>
-      <c r="C17" s="134"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="143"/>
+      <c r="B17" s="154"/>
+      <c r="C17" s="155"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="145"/>
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
       <c r="H17" s="54" t="s">
@@ -3161,16 +3213,16 @@
       <c r="J17" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="154"/>
+      <c r="K17" s="138"/>
     </row>
     <row r="18" spans="1:11" ht="10.5" customHeight="1">
       <c r="A18" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="133"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="142"/>
-      <c r="E18" s="143"/>
+      <c r="B18" s="154"/>
+      <c r="C18" s="155"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="145"/>
       <c r="F18" s="52"/>
       <c r="G18" s="67"/>
       <c r="H18" s="62" t="s">
@@ -3180,16 +3232,16 @@
         <v>33</v>
       </c>
       <c r="J18" s="62"/>
-      <c r="K18" s="154"/>
+      <c r="K18" s="138"/>
     </row>
     <row r="19" spans="1:11" ht="10.5" customHeight="1">
       <c r="A19" s="55">
         <v>921</v>
       </c>
-      <c r="B19" s="135"/>
-      <c r="C19" s="136"/>
-      <c r="D19" s="144"/>
-      <c r="E19" s="145"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="157"/>
+      <c r="D19" s="146"/>
+      <c r="E19" s="147"/>
       <c r="F19" s="56"/>
       <c r="G19" s="68"/>
       <c r="H19" s="54">
@@ -3199,24 +3251,24 @@
         <v>43814</v>
       </c>
       <c r="J19" s="50"/>
-      <c r="K19" s="154"/>
+      <c r="K19" s="138"/>
     </row>
     <row r="20" spans="1:11" ht="10.5" customHeight="1">
       <c r="A20" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="158" t="s">
+      <c r="B20" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="158"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="156"/>
-      <c r="F20" s="156"/>
-      <c r="G20" s="156"/>
-      <c r="H20" s="156"/>
-      <c r="I20" s="156"/>
-      <c r="J20" s="156"/>
-      <c r="K20" s="156"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="129"/>
+      <c r="E20" s="129"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="129"/>
+      <c r="J20" s="129"/>
+      <c r="K20" s="129"/>
     </row>
     <row r="21" spans="1:11" ht="10.5" customHeight="1">
       <c r="A21" s="110" t="s">
@@ -3239,22 +3291,22 @@
       <c r="A22" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="138" t="s">
+      <c r="B22" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="139"/>
-      <c r="D22" s="138" t="s">
+      <c r="C22" s="136"/>
+      <c r="D22" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="139"/>
-      <c r="F22" s="138" t="s">
+      <c r="E22" s="136"/>
+      <c r="F22" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="139"/>
-      <c r="H22" s="137" t="s">
+      <c r="G22" s="136"/>
+      <c r="H22" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="137"/>
+      <c r="I22" s="158"/>
       <c r="J22" s="62" t="s">
         <v>30</v>
       </c>
@@ -3267,35 +3319,35 @@
         <f>A15+1</f>
         <v>3</v>
       </c>
-      <c r="B23" s="131" t="s">
+      <c r="B23" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="132"/>
-      <c r="D23" s="140" t="s">
+      <c r="C23" s="153"/>
+      <c r="D23" s="142" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="141"/>
-      <c r="F23" s="140" t="s">
+      <c r="E23" s="143"/>
+      <c r="F23" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="G23" s="141"/>
-      <c r="H23" s="146" t="s">
+      <c r="G23" s="143"/>
+      <c r="H23" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="147"/>
+      <c r="I23" s="141"/>
       <c r="J23" s="50"/>
-      <c r="K23" s="153"/>
+      <c r="K23" s="137"/>
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="133"/>
-      <c r="C24" s="134"/>
-      <c r="D24" s="142"/>
-      <c r="E24" s="143"/>
-      <c r="F24" s="142"/>
-      <c r="G24" s="143"/>
+      <c r="B24" s="154"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="145"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="145"/>
       <c r="H24" s="62" t="s">
         <v>34</v>
       </c>
@@ -3305,18 +3357,18 @@
       <c r="J24" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="154"/>
+      <c r="K24" s="138"/>
     </row>
     <row r="25" spans="1:11" ht="10.5" customHeight="1">
       <c r="A25" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="133"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="142"/>
-      <c r="E25" s="143"/>
-      <c r="F25" s="142"/>
-      <c r="G25" s="143"/>
+      <c r="B25" s="154"/>
+      <c r="C25" s="155"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="144"/>
+      <c r="G25" s="145"/>
       <c r="H25" s="54" t="s">
         <v>61</v>
       </c>
@@ -3324,35 +3376,35 @@
         <v>62</v>
       </c>
       <c r="J25" s="50"/>
-      <c r="K25" s="154"/>
+      <c r="K25" s="138"/>
     </row>
     <row r="26" spans="1:11" ht="10.5" customHeight="1">
       <c r="A26" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="133"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="142"/>
-      <c r="E26" s="143"/>
-      <c r="F26" s="142"/>
-      <c r="G26" s="143"/>
+      <c r="B26" s="154"/>
+      <c r="C26" s="155"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="145"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="145"/>
       <c r="H26" s="62" t="s">
         <v>36</v>
       </c>
       <c r="I26" s="62"/>
       <c r="J26" s="62"/>
-      <c r="K26" s="154"/>
+      <c r="K26" s="138"/>
     </row>
     <row r="27" spans="1:11" ht="10.5" customHeight="1">
       <c r="A27" s="55">
         <v>922</v>
       </c>
-      <c r="B27" s="135"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="144"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="144"/>
-      <c r="G27" s="145"/>
+      <c r="B27" s="156"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="146"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="146"/>
+      <c r="G27" s="147"/>
       <c r="H27" s="54">
         <v>43813</v>
       </c>
@@ -3360,28 +3412,28 @@
         <v>43813</v>
       </c>
       <c r="J27" s="50"/>
-      <c r="K27" s="155"/>
+      <c r="K27" s="139"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="129" t="s">
+      <c r="B28" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="130"/>
-      <c r="D28" s="129" t="s">
+      <c r="C28" s="133"/>
+      <c r="D28" s="132" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="130"/>
-      <c r="F28" s="129" t="s">
+      <c r="E28" s="133"/>
+      <c r="F28" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="130"/>
-      <c r="H28" s="152" t="s">
+      <c r="G28" s="133"/>
+      <c r="H28" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="152"/>
+      <c r="I28" s="130"/>
       <c r="J28" s="47" t="s">
         <v>30</v>
       </c>
@@ -3393,35 +3445,35 @@
       <c r="A29" s="50">
         <v>4</v>
       </c>
-      <c r="B29" s="131" t="s">
+      <c r="B29" s="152" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="132"/>
-      <c r="D29" s="140" t="s">
+      <c r="C29" s="153"/>
+      <c r="D29" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="141"/>
-      <c r="F29" s="140" t="s">
+      <c r="E29" s="143"/>
+      <c r="F29" s="142" t="s">
         <v>65</v>
       </c>
-      <c r="G29" s="141"/>
+      <c r="G29" s="143"/>
       <c r="H29" s="148" t="s">
         <v>38</v>
       </c>
       <c r="I29" s="149"/>
       <c r="J29" s="57"/>
-      <c r="K29" s="153"/>
+      <c r="K29" s="137"/>
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="133"/>
-      <c r="C30" s="134"/>
-      <c r="D30" s="142"/>
-      <c r="E30" s="143"/>
-      <c r="F30" s="142"/>
-      <c r="G30" s="143"/>
+      <c r="B30" s="154"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="144"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="145"/>
       <c r="H30" s="47" t="s">
         <v>34</v>
       </c>
@@ -3431,18 +3483,18 @@
       <c r="J30" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="154"/>
+      <c r="K30" s="138"/>
     </row>
     <row r="31" spans="1:11" ht="10.5" customHeight="1">
       <c r="A31" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="133"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="142"/>
-      <c r="E31" s="143"/>
-      <c r="F31" s="142"/>
-      <c r="G31" s="143"/>
+      <c r="B31" s="154"/>
+      <c r="C31" s="155"/>
+      <c r="D31" s="144"/>
+      <c r="E31" s="145"/>
+      <c r="F31" s="144"/>
+      <c r="G31" s="145"/>
       <c r="H31" s="54" t="s">
         <v>61</v>
       </c>
@@ -3450,18 +3502,18 @@
         <v>62</v>
       </c>
       <c r="J31" s="50"/>
-      <c r="K31" s="154"/>
+      <c r="K31" s="138"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="133"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="142"/>
-      <c r="E32" s="143"/>
-      <c r="F32" s="142"/>
-      <c r="G32" s="143"/>
+      <c r="B32" s="154"/>
+      <c r="C32" s="155"/>
+      <c r="D32" s="144"/>
+      <c r="E32" s="145"/>
+      <c r="F32" s="144"/>
+      <c r="G32" s="145"/>
       <c r="H32" s="47" t="s">
         <v>36</v>
       </c>
@@ -3469,18 +3521,18 @@
         <v>33</v>
       </c>
       <c r="J32" s="47"/>
-      <c r="K32" s="154"/>
+      <c r="K32" s="138"/>
     </row>
     <row r="33" spans="1:11" ht="10.5" customHeight="1">
       <c r="A33" s="55">
         <v>823</v>
       </c>
-      <c r="B33" s="135"/>
-      <c r="C33" s="136"/>
-      <c r="D33" s="144"/>
-      <c r="E33" s="145"/>
-      <c r="F33" s="144"/>
-      <c r="G33" s="145"/>
+      <c r="B33" s="156"/>
+      <c r="C33" s="157"/>
+      <c r="D33" s="146"/>
+      <c r="E33" s="147"/>
+      <c r="F33" s="146"/>
+      <c r="G33" s="147"/>
       <c r="H33" s="54">
         <v>43813</v>
       </c>
@@ -3488,28 +3540,28 @@
         <v>43814</v>
       </c>
       <c r="J33" s="50"/>
-      <c r="K33" s="155"/>
+      <c r="K33" s="139"/>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="129" t="s">
+      <c r="B34" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="130"/>
-      <c r="D34" s="129" t="s">
+      <c r="C34" s="133"/>
+      <c r="D34" s="132" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="130"/>
-      <c r="F34" s="129" t="s">
+      <c r="E34" s="133"/>
+      <c r="F34" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="130"/>
-      <c r="H34" s="152" t="s">
+      <c r="G34" s="133"/>
+      <c r="H34" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="152"/>
+      <c r="I34" s="130"/>
       <c r="J34" s="47" t="s">
         <v>30</v>
       </c>
@@ -3521,35 +3573,35 @@
       <c r="A35" s="50">
         <v>5</v>
       </c>
-      <c r="B35" s="131" t="s">
+      <c r="B35" s="152" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="132"/>
-      <c r="D35" s="140" t="s">
+      <c r="C35" s="153"/>
+      <c r="D35" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="141"/>
-      <c r="F35" s="140" t="s">
+      <c r="E35" s="143"/>
+      <c r="F35" s="142" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="141"/>
+      <c r="G35" s="143"/>
       <c r="H35" s="148" t="s">
         <v>38</v>
       </c>
       <c r="I35" s="149"/>
       <c r="J35" s="57"/>
-      <c r="K35" s="153"/>
+      <c r="K35" s="137"/>
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="133"/>
-      <c r="C36" s="134"/>
-      <c r="D36" s="142"/>
-      <c r="E36" s="143"/>
-      <c r="F36" s="142"/>
-      <c r="G36" s="143"/>
+      <c r="B36" s="154"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="144"/>
+      <c r="E36" s="145"/>
+      <c r="F36" s="144"/>
+      <c r="G36" s="145"/>
       <c r="H36" s="47" t="s">
         <v>34</v>
       </c>
@@ -3559,18 +3611,18 @@
       <c r="J36" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="154"/>
+      <c r="K36" s="138"/>
     </row>
     <row r="37" spans="1:11" ht="10.5" customHeight="1">
       <c r="A37" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="133"/>
-      <c r="C37" s="134"/>
-      <c r="D37" s="142"/>
-      <c r="E37" s="143"/>
-      <c r="F37" s="142"/>
-      <c r="G37" s="143"/>
+      <c r="B37" s="154"/>
+      <c r="C37" s="155"/>
+      <c r="D37" s="144"/>
+      <c r="E37" s="145"/>
+      <c r="F37" s="144"/>
+      <c r="G37" s="145"/>
       <c r="H37" s="54" t="s">
         <v>61</v>
       </c>
@@ -3578,18 +3630,18 @@
         <v>62</v>
       </c>
       <c r="J37" s="50"/>
-      <c r="K37" s="154"/>
+      <c r="K37" s="138"/>
     </row>
     <row r="38" spans="1:11" ht="10.5" customHeight="1">
       <c r="A38" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="133"/>
-      <c r="C38" s="134"/>
-      <c r="D38" s="142"/>
-      <c r="E38" s="143"/>
-      <c r="F38" s="142"/>
-      <c r="G38" s="143"/>
+      <c r="B38" s="154"/>
+      <c r="C38" s="155"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="145"/>
+      <c r="F38" s="144"/>
+      <c r="G38" s="145"/>
       <c r="H38" s="47" t="s">
         <v>36</v>
       </c>
@@ -3597,18 +3649,18 @@
         <v>33</v>
       </c>
       <c r="J38" s="47"/>
-      <c r="K38" s="154"/>
+      <c r="K38" s="138"/>
     </row>
     <row r="39" spans="1:11" ht="10.5" customHeight="1">
       <c r="A39" s="55">
         <v>823</v>
       </c>
-      <c r="B39" s="135"/>
-      <c r="C39" s="136"/>
-      <c r="D39" s="144"/>
-      <c r="E39" s="145"/>
-      <c r="F39" s="144"/>
-      <c r="G39" s="145"/>
+      <c r="B39" s="156"/>
+      <c r="C39" s="157"/>
+      <c r="D39" s="146"/>
+      <c r="E39" s="147"/>
+      <c r="F39" s="146"/>
+      <c r="G39" s="147"/>
       <c r="H39" s="54">
         <v>43813</v>
       </c>
@@ -3616,7 +3668,7 @@
         <v>43814</v>
       </c>
       <c r="J39" s="50"/>
-      <c r="K39" s="155"/>
+      <c r="K39" s="139"/>
     </row>
     <row r="40" spans="1:11" s="65" customFormat="1">
       <c r="A40" s="72"/>
@@ -4019,6 +4071,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C13"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C27"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B29:C33"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B35:C39"/>
+    <mergeCell ref="D29:E33"/>
+    <mergeCell ref="D35:E39"/>
+    <mergeCell ref="F35:G39"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="D15:E19"/>
+    <mergeCell ref="B15:C19"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="F29:G33"/>
+    <mergeCell ref="K29:K33"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H8:I8"/>
@@ -4035,36 +4117,6 @@
     <mergeCell ref="D23:E27"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="F23:G27"/>
-    <mergeCell ref="K35:K39"/>
-    <mergeCell ref="F29:G33"/>
-    <mergeCell ref="K29:K33"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="D15:E19"/>
-    <mergeCell ref="B15:C19"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B35:C39"/>
-    <mergeCell ref="D29:E33"/>
-    <mergeCell ref="D35:E39"/>
-    <mergeCell ref="F35:G39"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C27"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B29:C33"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C13"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H35:I35">

</xml_diff>

<commit_message>
Thêm thông tin Công ty và logo
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="78">
   <si>
     <t>Online ID</t>
   </si>
@@ -273,9 +273,6 @@
     <t>Approval:</t>
   </si>
   <si>
-    <t>Name and Organization</t>
-  </si>
-  <si>
     <t>Concurrence:</t>
   </si>
   <si>
@@ -430,6 +427,12 @@
   </si>
   <si>
     <t>Tài liệu môn quản trị dự án - Tiến NĐ</t>
+  </si>
+  <si>
+    <t>H3B</t>
+  </si>
+  <si>
+    <t>H3B CEO</t>
   </si>
 </sst>
 </file>
@@ -1770,8 +1773,8 @@
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -1816,7 +1819,7 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -1935,7 +1938,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -1990,11 +1993,11 @@
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
@@ -2084,10 +2087,10 @@
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="81" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F15" s="81"/>
       <c r="G15" s="81"/>
@@ -2269,10 +2272,10 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2298,7 +2301,7 @@
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="L24" s="124" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M24" s="114"/>
       <c r="N24" s="114"/>
@@ -2469,7 +2472,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2539,7 +2542,7 @@
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
       <c r="C34" s="39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -2575,7 +2578,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2857,7 +2860,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="65" customFormat="1">
       <c r="A1" s="87" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="88" t="str">
         <f>Overview!E9</f>
@@ -2868,26 +2871,26 @@
       <c r="E1" s="89"/>
       <c r="F1" s="89"/>
       <c r="G1" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="91" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" s="91" t="s">
-        <v>46</v>
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
         <v>4</v>
       </c>
       <c r="J1" s="92" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K1" s="93"/>
     </row>
     <row r="2" spans="1:11" s="65" customFormat="1">
       <c r="A2" s="126" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="95"/>
@@ -2895,23 +2898,23 @@
       <c r="F2" s="96"/>
       <c r="G2" s="97"/>
       <c r="H2" s="98" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="112">
         <f>COUNTIF(H2:H787,"Not OK")</f>
         <v>1</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
       <c r="A3" s="94" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="95"/>
       <c r="D3" s="95"/>
@@ -2919,14 +2922,14 @@
       <c r="F3" s="96"/>
       <c r="G3" s="97"/>
       <c r="H3" s="98" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="113">
         <f>COUNTIF(H2:H787,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="99" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K3" s="100"/>
     </row>
@@ -2938,7 +2941,7 @@
       <c r="E4" s="96"/>
       <c r="F4" s="96"/>
       <c r="G4" s="102" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" s="95"/>
       <c r="I4" s="112">
@@ -2993,29 +2996,29 @@
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="132" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="132" t="s">
-        <v>27</v>
       </c>
       <c r="C8" s="133"/>
       <c r="D8" s="132" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="133"/>
       <c r="F8" s="132" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="133"/>
       <c r="H8" s="131" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="131"/>
       <c r="J8" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="49" t="s">
         <v>30</v>
-      </c>
-      <c r="K8" s="49" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
@@ -3023,19 +3026,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="152" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="153"/>
       <c r="D9" s="142" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="143"/>
       <c r="F9" s="51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="140" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="141"/>
       <c r="J9" s="50"/>
@@ -3043,7 +3046,7 @@
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="154"/>
       <c r="C10" s="155"/>
@@ -3052,13 +3055,13 @@
       <c r="F10" s="52"/>
       <c r="G10" s="67"/>
       <c r="H10" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K10" s="138"/>
     </row>
@@ -3073,10 +3076,10 @@
       <c r="F11" s="52"/>
       <c r="G11" s="67"/>
       <c r="H11" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="54" t="s">
         <v>61</v>
-      </c>
-      <c r="I11" s="54" t="s">
-        <v>62</v>
       </c>
       <c r="J11" s="50"/>
       <c r="K11" s="138"/>
@@ -3092,10 +3095,10 @@
       <c r="F12" s="52"/>
       <c r="G12" s="67"/>
       <c r="H12" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J12" s="47"/>
       <c r="K12" s="138"/>
@@ -3121,29 +3124,29 @@
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="135" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="136"/>
       <c r="D14" s="135" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="136"/>
       <c r="F14" s="135" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G14" s="136"/>
       <c r="H14" s="158" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="158"/>
       <c r="J14" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="61" t="s">
         <v>30</v>
-      </c>
-      <c r="K14" s="61" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="10.5" customHeight="1">
@@ -3151,31 +3154,31 @@
         <v>2</v>
       </c>
       <c r="B15" s="152" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="153"/>
       <c r="D15" s="142" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="143"/>
       <c r="F15" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G15" s="66"/>
       <c r="H15" s="148" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" s="149"/>
       <c r="J15" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K15" s="137" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="154"/>
       <c r="C16" s="155"/>
@@ -3184,13 +3187,13 @@
       <c r="F16" s="52"/>
       <c r="G16" s="67"/>
       <c r="H16" s="62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K16" s="138"/>
     </row>
@@ -3205,13 +3208,13 @@
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
       <c r="H17" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="I17" s="54" t="s">
-        <v>62</v>
-      </c>
       <c r="J17" s="50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K17" s="138"/>
     </row>
@@ -3226,10 +3229,10 @@
       <c r="F18" s="52"/>
       <c r="G18" s="67"/>
       <c r="H18" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="138"/>
@@ -3289,29 +3292,29 @@
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A22" s="62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="135" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="136"/>
       <c r="D22" s="135" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="136"/>
       <c r="F22" s="135" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G22" s="136"/>
       <c r="H22" s="158" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I22" s="158"/>
       <c r="J22" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="62" t="s">
         <v>30</v>
-      </c>
-      <c r="K22" s="62" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
@@ -3320,19 +3323,19 @@
         <v>3</v>
       </c>
       <c r="B23" s="152" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="153"/>
       <c r="D23" s="142" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E23" s="143"/>
       <c r="F23" s="142" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G23" s="143"/>
       <c r="H23" s="140" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I23" s="141"/>
       <c r="J23" s="50"/>
@@ -3340,7 +3343,7 @@
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="154"/>
       <c r="C24" s="155"/>
@@ -3349,13 +3352,13 @@
       <c r="F24" s="144"/>
       <c r="G24" s="145"/>
       <c r="H24" s="62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I24" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K24" s="138"/>
     </row>
@@ -3370,10 +3373,10 @@
       <c r="F25" s="144"/>
       <c r="G25" s="145"/>
       <c r="H25" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="54" t="s">
         <v>61</v>
-      </c>
-      <c r="I25" s="54" t="s">
-        <v>62</v>
       </c>
       <c r="J25" s="50"/>
       <c r="K25" s="138"/>
@@ -3389,7 +3392,7 @@
       <c r="F26" s="144"/>
       <c r="G26" s="145"/>
       <c r="H26" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I26" s="62"/>
       <c r="J26" s="62"/>
@@ -3416,29 +3419,29 @@
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="132" t="s">
         <v>26</v>
-      </c>
-      <c r="B28" s="132" t="s">
-        <v>27</v>
       </c>
       <c r="C28" s="133"/>
       <c r="D28" s="132" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="133"/>
       <c r="F28" s="132" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G28" s="133"/>
       <c r="H28" s="130" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I28" s="130"/>
       <c r="J28" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28" s="63" t="s">
         <v>30</v>
-      </c>
-      <c r="K28" s="63" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
@@ -3446,19 +3449,19 @@
         <v>4</v>
       </c>
       <c r="B29" s="152" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="153"/>
       <c r="D29" s="142" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" s="143"/>
       <c r="F29" s="142" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G29" s="143"/>
       <c r="H29" s="148" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I29" s="149"/>
       <c r="J29" s="57"/>
@@ -3466,7 +3469,7 @@
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="154"/>
       <c r="C30" s="155"/>
@@ -3475,13 +3478,13 @@
       <c r="F30" s="144"/>
       <c r="G30" s="145"/>
       <c r="H30" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I30" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J30" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K30" s="138"/>
     </row>
@@ -3496,10 +3499,10 @@
       <c r="F31" s="144"/>
       <c r="G31" s="145"/>
       <c r="H31" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="54" t="s">
         <v>61</v>
-      </c>
-      <c r="I31" s="54" t="s">
-        <v>62</v>
       </c>
       <c r="J31" s="50"/>
       <c r="K31" s="138"/>
@@ -3515,10 +3518,10 @@
       <c r="F32" s="144"/>
       <c r="G32" s="145"/>
       <c r="H32" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I32" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J32" s="47"/>
       <c r="K32" s="138"/>
@@ -3544,29 +3547,29 @@
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="132" t="s">
         <v>26</v>
-      </c>
-      <c r="B34" s="132" t="s">
-        <v>27</v>
       </c>
       <c r="C34" s="133"/>
       <c r="D34" s="132" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E34" s="133"/>
       <c r="F34" s="132" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G34" s="133"/>
       <c r="H34" s="130" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I34" s="130"/>
       <c r="J34" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="63" t="s">
         <v>30</v>
-      </c>
-      <c r="K34" s="63" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
@@ -3574,19 +3577,19 @@
         <v>5</v>
       </c>
       <c r="B35" s="152" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="153"/>
       <c r="D35" s="142" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E35" s="143"/>
       <c r="F35" s="142" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G35" s="143"/>
       <c r="H35" s="148" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I35" s="149"/>
       <c r="J35" s="57"/>
@@ -3594,7 +3597,7 @@
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="154"/>
       <c r="C36" s="155"/>
@@ -3603,13 +3606,13 @@
       <c r="F36" s="144"/>
       <c r="G36" s="145"/>
       <c r="H36" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I36" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J36" s="47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K36" s="138"/>
     </row>
@@ -3624,10 +3627,10 @@
       <c r="F37" s="144"/>
       <c r="G37" s="145"/>
       <c r="H37" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="I37" s="54" t="s">
         <v>61</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>62</v>
       </c>
       <c r="J37" s="50"/>
       <c r="K37" s="138"/>
@@ -3643,10 +3646,10 @@
       <c r="F38" s="144"/>
       <c r="G38" s="145"/>
       <c r="H38" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I38" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J38" s="47"/>
       <c r="K38" s="138"/>

</xml_diff>

<commit_message>
Check lỗi chính tả
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -423,9 +423,6 @@
     <t>Kiểm tra các lỗi như SQL Injection,..</t>
   </si>
   <si>
-    <t>MySQL, AWS,...</t>
-  </si>
-  <si>
     <t>Tài liệu môn quản trị dự án - Tiến NĐ</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>H3B CEO</t>
+  </si>
+  <si>
+    <t>MySQL, AWS, ...</t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1774,7 @@
   <dimension ref="A1:AI44"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -2090,7 +2090,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F15" s="81"/>
       <c r="G15" s="81"/>
@@ -2275,7 +2275,7 @@
         <v>39</v>
       </c>
       <c r="E22" s="81" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2472,7 +2472,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2578,7 +2578,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>

</xml_diff>

<commit_message>
Kiểm tra lần cuối
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_Testcase.xlsx
+++ b/docs/ProjectCode_Testcase.xlsx
@@ -240,9 +240,6 @@
     <t>1.2.2-2</t>
   </si>
   <si>
-    <t>Test case Overview</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Project Name:</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>MySQL, AWS, ...</t>
+  </si>
+  <si>
+    <t>Test case Overview H3B Company</t>
   </si>
 </sst>
 </file>
@@ -1773,8 +1773,8 @@
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.25"/>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="5"/>
@@ -1901,7 +1901,7 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
       <c r="O6" s="127" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="P6" s="127"/>
       <c r="Q6" s="127"/>
@@ -1935,10 +1935,10 @@
       <c r="B9" s="30"/>
       <c r="C9" s="18"/>
       <c r="D9" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -1949,7 +1949,7 @@
       <c r="B10" s="30"/>
       <c r="C10" s="18"/>
       <c r="D10" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="28">
         <v>1</v>
@@ -1961,7 +1961,7 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
       <c r="L10" s="124" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
@@ -1975,7 +1975,7 @@
       <c r="B11" s="30"/>
       <c r="C11" s="18"/>
       <c r="D11" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="128">
         <v>43831</v>
@@ -1984,24 +1984,24 @@
       <c r="G11" s="128"/>
       <c r="H11" s="82"/>
       <c r="L11" s="33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M11" s="33"/>
       <c r="N11" s="33"/>
       <c r="O11" s="33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R11" s="33"/>
       <c r="S11" s="33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T11" s="33"/>
       <c r="U11" s="33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V11" s="33"/>
       <c r="X11" s="19"/>
@@ -2009,7 +2009,7 @@
     <row r="12" spans="1:24">
       <c r="B12" s="30"/>
       <c r="L12" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
@@ -2087,10 +2087,10 @@
     <row r="15" spans="1:24">
       <c r="B15" s="30"/>
       <c r="D15" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="81"/>
       <c r="G15" s="81"/>
@@ -2220,7 +2220,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
       <c r="L19" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
@@ -2272,10 +2272,10 @@
       <c r="B22" s="15"/>
       <c r="C22" s="4"/>
       <c r="D22" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F22" s="81"/>
       <c r="G22" s="81"/>
@@ -2301,7 +2301,7 @@
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="L24" s="124" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M24" s="114"/>
       <c r="N24" s="114"/>
@@ -2436,7 +2436,7 @@
     <row r="31" spans="2:35">
       <c r="B31" s="15"/>
       <c r="C31" s="39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="28"/>
@@ -2472,7 +2472,7 @@
     <row r="32" spans="2:35">
       <c r="B32" s="46"/>
       <c r="C32" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -2542,7 +2542,7 @@
     <row r="34" spans="1:35">
       <c r="B34" s="30"/>
       <c r="C34" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="28"/>
@@ -2578,7 +2578,7 @@
     <row r="35" spans="1:35">
       <c r="B35" s="30"/>
       <c r="C35" s="40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
@@ -2845,8 +2845,8 @@
   </sheetPr>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B14" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2860,7 +2860,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="65" customFormat="1">
       <c r="A1" s="87" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="88" t="str">
         <f>Overview!E9</f>
@@ -2871,26 +2871,26 @@
       <c r="E1" s="89"/>
       <c r="F1" s="89"/>
       <c r="G1" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="91" t="s">
         <v>44</v>
-      </c>
-      <c r="H1" s="91" t="s">
-        <v>45</v>
       </c>
       <c r="I1" s="111">
         <f>COUNTIF(H1:H786,"OK")</f>
         <v>4</v>
       </c>
       <c r="J1" s="92" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K1" s="93"/>
     </row>
     <row r="2" spans="1:11" s="65" customFormat="1">
       <c r="A2" s="126" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="95"/>
@@ -2898,23 +2898,23 @@
       <c r="F2" s="96"/>
       <c r="G2" s="97"/>
       <c r="H2" s="98" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="112">
         <f>COUNTIF(H2:H787,"Not OK")</f>
         <v>1</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:11" s="65" customFormat="1" ht="11.25" customHeight="1">
       <c r="A3" s="94" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="95" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="95"/>
       <c r="D3" s="95"/>
@@ -2922,14 +2922,14 @@
       <c r="F3" s="96"/>
       <c r="G3" s="97"/>
       <c r="H3" s="98" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="113">
         <f>COUNTIF(H2:H787,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3" s="100"/>
     </row>
@@ -2941,7 +2941,7 @@
       <c r="E4" s="96"/>
       <c r="F4" s="96"/>
       <c r="G4" s="102" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="95"/>
       <c r="I4" s="112">
@@ -2996,29 +2996,29 @@
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="132" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" s="132" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="133"/>
       <c r="D8" s="132" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="133"/>
       <c r="F8" s="132" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="133"/>
       <c r="H8" s="131" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="131"/>
       <c r="J8" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="49" t="s">
         <v>29</v>
-      </c>
-      <c r="K8" s="49" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="10.5" customHeight="1">
@@ -3026,19 +3026,19 @@
         <v>1</v>
       </c>
       <c r="B9" s="152" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="153"/>
       <c r="D9" s="142" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="143"/>
       <c r="F9" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="66"/>
       <c r="H9" s="140" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" s="141"/>
       <c r="J9" s="50"/>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="10" spans="1:11" ht="10.5" customHeight="1">
       <c r="A10" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="154"/>
       <c r="C10" s="155"/>
@@ -3055,13 +3055,13 @@
       <c r="F10" s="52"/>
       <c r="G10" s="67"/>
       <c r="H10" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" s="138"/>
     </row>
@@ -3076,10 +3076,10 @@
       <c r="F11" s="52"/>
       <c r="G11" s="67"/>
       <c r="H11" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="54" t="s">
         <v>60</v>
-      </c>
-      <c r="I11" s="54" t="s">
-        <v>61</v>
       </c>
       <c r="J11" s="50"/>
       <c r="K11" s="138"/>
@@ -3095,10 +3095,10 @@
       <c r="F12" s="52"/>
       <c r="G12" s="67"/>
       <c r="H12" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12" s="47"/>
       <c r="K12" s="138"/>
@@ -3124,29 +3124,29 @@
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A14" s="60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="135" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="136"/>
       <c r="D14" s="135" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" s="136"/>
       <c r="F14" s="135" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="136"/>
       <c r="H14" s="158" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14" s="158"/>
       <c r="J14" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="61" t="s">
         <v>29</v>
-      </c>
-      <c r="K14" s="61" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="10.5" customHeight="1">
@@ -3154,31 +3154,31 @@
         <v>2</v>
       </c>
       <c r="B15" s="152" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="153"/>
       <c r="D15" s="142" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" s="143"/>
       <c r="F15" s="51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="66"/>
       <c r="H15" s="148" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="149"/>
       <c r="J15" s="57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K15" s="137" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="154"/>
       <c r="C16" s="155"/>
@@ -3187,13 +3187,13 @@
       <c r="F16" s="52"/>
       <c r="G16" s="67"/>
       <c r="H16" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="138"/>
     </row>
@@ -3208,13 +3208,13 @@
       <c r="F17" s="52"/>
       <c r="G17" s="67"/>
       <c r="H17" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="54" t="s">
-        <v>61</v>
-      </c>
       <c r="J17" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K17" s="138"/>
     </row>
@@ -3229,10 +3229,10 @@
       <c r="F18" s="52"/>
       <c r="G18" s="67"/>
       <c r="H18" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18" s="62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J18" s="62"/>
       <c r="K18" s="138"/>
@@ -3292,29 +3292,29 @@
     </row>
     <row r="22" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A22" s="62" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="135" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="136"/>
       <c r="D22" s="135" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="136"/>
       <c r="F22" s="135" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G22" s="136"/>
       <c r="H22" s="158" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I22" s="158"/>
       <c r="J22" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="62" t="s">
         <v>29</v>
-      </c>
-      <c r="K22" s="62" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="10.5" customHeight="1">
@@ -3323,19 +3323,19 @@
         <v>3</v>
       </c>
       <c r="B23" s="152" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="153"/>
       <c r="D23" s="142" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" s="143"/>
       <c r="F23" s="142" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" s="143"/>
       <c r="H23" s="140" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I23" s="141"/>
       <c r="J23" s="50"/>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="24" spans="1:11" ht="10.5" customHeight="1">
       <c r="A24" s="62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="154"/>
       <c r="C24" s="155"/>
@@ -3352,13 +3352,13 @@
       <c r="F24" s="144"/>
       <c r="G24" s="145"/>
       <c r="H24" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I24" s="62" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K24" s="138"/>
     </row>
@@ -3373,10 +3373,10 @@
       <c r="F25" s="144"/>
       <c r="G25" s="145"/>
       <c r="H25" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="54" t="s">
         <v>60</v>
-      </c>
-      <c r="I25" s="54" t="s">
-        <v>61</v>
       </c>
       <c r="J25" s="50"/>
       <c r="K25" s="138"/>
@@ -3392,7 +3392,7 @@
       <c r="F26" s="144"/>
       <c r="G26" s="145"/>
       <c r="H26" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I26" s="62"/>
       <c r="J26" s="62"/>
@@ -3419,29 +3419,29 @@
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A28" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="132" t="s">
         <v>25</v>
-      </c>
-      <c r="B28" s="132" t="s">
-        <v>26</v>
       </c>
       <c r="C28" s="133"/>
       <c r="D28" s="132" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E28" s="133"/>
       <c r="F28" s="132" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" s="133"/>
       <c r="H28" s="130" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I28" s="130"/>
       <c r="J28" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="63" t="s">
         <v>29</v>
-      </c>
-      <c r="K28" s="63" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="10.5" customHeight="1">
@@ -3449,19 +3449,19 @@
         <v>4</v>
       </c>
       <c r="B29" s="152" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="153"/>
       <c r="D29" s="142" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E29" s="143"/>
       <c r="F29" s="142" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G29" s="143"/>
       <c r="H29" s="148" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I29" s="149"/>
       <c r="J29" s="57"/>
@@ -3469,7 +3469,7 @@
     </row>
     <row r="30" spans="1:11" ht="10.5" customHeight="1">
       <c r="A30" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="154"/>
       <c r="C30" s="155"/>
@@ -3478,13 +3478,13 @@
       <c r="F30" s="144"/>
       <c r="G30" s="145"/>
       <c r="H30" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I30" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J30" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K30" s="138"/>
     </row>
@@ -3499,10 +3499,10 @@
       <c r="F31" s="144"/>
       <c r="G31" s="145"/>
       <c r="H31" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="54" t="s">
         <v>60</v>
-      </c>
-      <c r="I31" s="54" t="s">
-        <v>61</v>
       </c>
       <c r="J31" s="50"/>
       <c r="K31" s="138"/>
@@ -3518,10 +3518,10 @@
       <c r="F32" s="144"/>
       <c r="G32" s="145"/>
       <c r="H32" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I32" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J32" s="47"/>
       <c r="K32" s="138"/>
@@ -3547,29 +3547,29 @@
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A34" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="132" t="s">
         <v>25</v>
-      </c>
-      <c r="B34" s="132" t="s">
-        <v>26</v>
       </c>
       <c r="C34" s="133"/>
       <c r="D34" s="132" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E34" s="133"/>
       <c r="F34" s="132" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G34" s="133"/>
       <c r="H34" s="130" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I34" s="130"/>
       <c r="J34" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="63" t="s">
         <v>29</v>
-      </c>
-      <c r="K34" s="63" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
@@ -3577,19 +3577,19 @@
         <v>5</v>
       </c>
       <c r="B35" s="152" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="153"/>
       <c r="D35" s="142" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E35" s="143"/>
       <c r="F35" s="142" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G35" s="143"/>
       <c r="H35" s="148" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I35" s="149"/>
       <c r="J35" s="57"/>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="36" spans="1:11" ht="10.5" customHeight="1">
       <c r="A36" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="154"/>
       <c r="C36" s="155"/>
@@ -3606,13 +3606,13 @@
       <c r="F36" s="144"/>
       <c r="G36" s="145"/>
       <c r="H36" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I36" s="47" t="s">
         <v>1</v>
       </c>
       <c r="J36" s="47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K36" s="138"/>
     </row>
@@ -3627,10 +3627,10 @@
       <c r="F37" s="144"/>
       <c r="G37" s="145"/>
       <c r="H37" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="I37" s="54" t="s">
         <v>60</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>61</v>
       </c>
       <c r="J37" s="50"/>
       <c r="K37" s="138"/>
@@ -3646,10 +3646,10 @@
       <c r="F38" s="144"/>
       <c r="G38" s="145"/>
       <c r="H38" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I38" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J38" s="47"/>
       <c r="K38" s="138"/>

</xml_diff>